<commit_message>
Improvements to RND and extended RAM to 16 blocks
</commit_message>
<xml_diff>
--- a/block_builder/blocks.xlsx
+++ b/block_builder/blocks.xlsx
@@ -16,7 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -27,8 +27,16 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FFEFEFEF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF1C4587"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -49,14 +57,74 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD6DCE4"/>
         <bgColor rgb="FFD6DCE4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8497B0"/>
-        <bgColor rgb="FF8497B0"/>
+        <fgColor rgb="FFE69138"/>
+        <bgColor rgb="FFE69138"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3C78D8"/>
+        <bgColor rgb="FF3C78D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF85200C"/>
+        <bgColor rgb="FF85200C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9900FF"/>
+        <bgColor rgb="FF9900FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA64D79"/>
+        <bgColor rgb="FFA64D79"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF38761D"/>
+        <bgColor rgb="FF38761D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor rgb="FF4A86E8"/>
       </patternFill>
     </fill>
   </fills>
@@ -143,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -175,22 +243,55 @@
     <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="8" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="7" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="0" fillId="15" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -553,14 +654,14 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
@@ -570,12 +671,12 @@
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="11"/>
-      <c r="AG7" s="11"/>
-      <c r="AH7" s="11"/>
-      <c r="AI7" s="11"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="6"/>
       <c r="AL7" s="6"/>
@@ -595,26 +696,26 @@
       <c r="AZ7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="12"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
@@ -624,12 +725,12 @@
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="11"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="6"/>
       <c r="AL8" s="6"/>
@@ -649,26 +750,26 @@
       <c r="AZ8" s="4"/>
     </row>
     <row r="9">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="11"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -678,12 +779,12 @@
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="6"/>
       <c r="AL9" s="6"/>
@@ -691,39 +792,39 @@
       <c r="AN9" s="6"/>
       <c r="AO9" s="6"/>
       <c r="AP9" s="6"/>
-      <c r="AQ9" s="11"/>
-      <c r="AR9" s="11"/>
-      <c r="AS9" s="11"/>
-      <c r="AT9" s="11"/>
-      <c r="AU9" s="11"/>
-      <c r="AV9" s="11"/>
-      <c r="AW9" s="11"/>
-      <c r="AX9" s="14"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="6"/>
+      <c r="AU9" s="6"/>
+      <c r="AV9" s="6"/>
+      <c r="AW9" s="6"/>
+      <c r="AX9" s="7"/>
       <c r="AY9" s="4"/>
       <c r="AZ9" s="4"/>
     </row>
     <row r="10">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
@@ -745,14 +846,14 @@
       <c r="AN10" s="6"/>
       <c r="AO10" s="6"/>
       <c r="AP10" s="6"/>
-      <c r="AQ10" s="11"/>
-      <c r="AR10" s="13"/>
-      <c r="AS10" s="13"/>
-      <c r="AT10" s="13"/>
-      <c r="AU10" s="13"/>
-      <c r="AV10" s="13"/>
-      <c r="AW10" s="13"/>
-      <c r="AX10" s="14"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="6"/>
+      <c r="AV10" s="6"/>
+      <c r="AW10" s="6"/>
+      <c r="AX10" s="7"/>
       <c r="AY10" s="4"/>
       <c r="AZ10" s="4"/>
     </row>
@@ -772,12 +873,12 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="11"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
@@ -799,14 +900,14 @@
       <c r="AN11" s="6"/>
       <c r="AO11" s="6"/>
       <c r="AP11" s="6"/>
-      <c r="AQ11" s="11"/>
-      <c r="AR11" s="11"/>
-      <c r="AS11" s="11"/>
-      <c r="AT11" s="11"/>
-      <c r="AU11" s="11"/>
-      <c r="AV11" s="11"/>
-      <c r="AW11" s="11"/>
-      <c r="AX11" s="14"/>
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="6"/>
+      <c r="AU11" s="6"/>
+      <c r="AV11" s="6"/>
+      <c r="AW11" s="6"/>
+      <c r="AX11" s="7"/>
       <c r="AY11" s="4"/>
       <c r="AZ11" s="4"/>
     </row>
@@ -826,12 +927,12 @@
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
       <c r="X12" s="9"/>
@@ -897,24 +998,24 @@
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AN13" s="11"/>
-      <c r="AO13" s="11"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="6"/>
+      <c r="AO13" s="6"/>
       <c r="AP13" s="6"/>
       <c r="AQ13" s="6"/>
       <c r="AR13" s="6"/>
       <c r="AS13" s="6"/>
       <c r="AT13" s="6"/>
       <c r="AU13" s="6"/>
-      <c r="AV13" s="11"/>
-      <c r="AW13" s="11"/>
-      <c r="AX13" s="14"/>
+      <c r="AV13" s="6"/>
+      <c r="AW13" s="6"/>
+      <c r="AX13" s="7"/>
       <c r="AY13" s="4"/>
       <c r="AZ13" s="4"/>
     </row>
@@ -924,21 +1025,21 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -951,24 +1052,24 @@
       <c r="AD14" s="6"/>
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="13"/>
-      <c r="AI14" s="13"/>
-      <c r="AJ14" s="13"/>
-      <c r="AK14" s="13"/>
-      <c r="AL14" s="13"/>
-      <c r="AM14" s="13"/>
-      <c r="AN14" s="13"/>
-      <c r="AO14" s="11"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
       <c r="AP14" s="6"/>
       <c r="AQ14" s="6"/>
       <c r="AR14" s="6"/>
       <c r="AS14" s="6"/>
       <c r="AT14" s="6"/>
       <c r="AU14" s="6"/>
-      <c r="AV14" s="11"/>
-      <c r="AW14" s="13"/>
-      <c r="AX14" s="14"/>
+      <c r="AV14" s="6"/>
+      <c r="AW14" s="6"/>
+      <c r="AX14" s="7"/>
       <c r="AY14" s="4"/>
       <c r="AZ14" s="4"/>
     </row>
@@ -978,21 +1079,21 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
@@ -1005,24 +1106,24 @@
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
       <c r="AF15" s="6"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="11"/>
-      <c r="AK15" s="11"/>
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="11"/>
-      <c r="AN15" s="11"/>
-      <c r="AO15" s="11"/>
-      <c r="AP15" s="6"/>
-      <c r="AQ15" s="6"/>
-      <c r="AR15" s="6"/>
-      <c r="AS15" s="6"/>
-      <c r="AT15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="6"/>
+      <c r="AL15" s="6"/>
+      <c r="AM15" s="13"/>
+      <c r="AN15" s="13"/>
+      <c r="AO15" s="13"/>
+      <c r="AP15" s="13"/>
+      <c r="AQ15" s="13"/>
+      <c r="AR15" s="13"/>
+      <c r="AS15" s="13"/>
+      <c r="AT15" s="13"/>
       <c r="AU15" s="6"/>
-      <c r="AV15" s="11"/>
-      <c r="AW15" s="13"/>
-      <c r="AX15" s="14"/>
+      <c r="AV15" s="6"/>
+      <c r="AW15" s="6"/>
+      <c r="AX15" s="7"/>
       <c r="AY15" s="4"/>
       <c r="AZ15" s="4"/>
     </row>
@@ -1032,28 +1133,28 @@
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
       <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
@@ -1065,18 +1166,18 @@
       <c r="AJ16" s="6"/>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
-      <c r="AM16" s="6"/>
-      <c r="AN16" s="6"/>
-      <c r="AO16" s="6"/>
-      <c r="AP16" s="6"/>
-      <c r="AQ16" s="6"/>
-      <c r="AR16" s="6"/>
-      <c r="AS16" s="6"/>
-      <c r="AT16" s="6"/>
+      <c r="AM16" s="13"/>
+      <c r="AN16" s="13"/>
+      <c r="AO16" s="13"/>
+      <c r="AP16" s="13"/>
+      <c r="AQ16" s="13"/>
+      <c r="AR16" s="13"/>
+      <c r="AS16" s="13"/>
+      <c r="AT16" s="13"/>
       <c r="AU16" s="6"/>
-      <c r="AV16" s="11"/>
-      <c r="AW16" s="11"/>
-      <c r="AX16" s="14"/>
+      <c r="AV16" s="6"/>
+      <c r="AW16" s="6"/>
+      <c r="AX16" s="7"/>
       <c r="AY16" s="4"/>
       <c r="AZ16" s="4"/>
     </row>
@@ -1101,13 +1202,13 @@
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="11"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
@@ -1119,14 +1220,14 @@
       <c r="AJ17" s="6"/>
       <c r="AK17" s="6"/>
       <c r="AL17" s="6"/>
-      <c r="AM17" s="6"/>
-      <c r="AN17" s="6"/>
-      <c r="AO17" s="6"/>
-      <c r="AP17" s="6"/>
-      <c r="AQ17" s="6"/>
-      <c r="AR17" s="6"/>
-      <c r="AS17" s="6"/>
-      <c r="AT17" s="6"/>
+      <c r="AM17" s="13"/>
+      <c r="AN17" s="13"/>
+      <c r="AO17" s="13"/>
+      <c r="AP17" s="13"/>
+      <c r="AQ17" s="13"/>
+      <c r="AR17" s="13"/>
+      <c r="AS17" s="13"/>
+      <c r="AT17" s="13"/>
       <c r="AU17" s="6"/>
       <c r="AV17" s="6"/>
       <c r="AW17" s="6"/>
@@ -1155,13 +1256,13 @@
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
       <c r="AD18" s="9"/>
@@ -1226,15 +1327,15 @@
       <c r="AI19" s="6"/>
       <c r="AJ19" s="6"/>
       <c r="AK19" s="6"/>
-      <c r="AL19" s="11"/>
-      <c r="AM19" s="11"/>
-      <c r="AN19" s="11"/>
-      <c r="AO19" s="11"/>
-      <c r="AP19" s="11"/>
-      <c r="AQ19" s="11"/>
-      <c r="AR19" s="11"/>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11"/>
+      <c r="AL19" s="6"/>
+      <c r="AM19" s="6"/>
+      <c r="AN19" s="6"/>
+      <c r="AO19" s="6"/>
+      <c r="AP19" s="6"/>
+      <c r="AQ19" s="6"/>
+      <c r="AR19" s="6"/>
+      <c r="AS19" s="6"/>
+      <c r="AT19" s="6"/>
       <c r="AU19" s="6"/>
       <c r="AV19" s="6"/>
       <c r="AW19" s="6"/>
@@ -1244,51 +1345,51 @@
     </row>
     <row r="20">
       <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11"/>
-      <c r="AB20" s="11"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
-      <c r="AE20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="14"/>
       <c r="AF20" s="6"/>
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="6"/>
       <c r="AK20" s="6"/>
-      <c r="AL20" s="11"/>
-      <c r="AM20" s="13"/>
-      <c r="AN20" s="13"/>
-      <c r="AO20" s="13"/>
-      <c r="AP20" s="13"/>
-      <c r="AQ20" s="13"/>
-      <c r="AR20" s="13"/>
-      <c r="AS20" s="13"/>
-      <c r="AT20" s="11"/>
+      <c r="AL20" s="6"/>
+      <c r="AM20" s="6"/>
+      <c r="AN20" s="6"/>
+      <c r="AO20" s="6"/>
+      <c r="AP20" s="6"/>
+      <c r="AQ20" s="6"/>
+      <c r="AR20" s="6"/>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="6"/>
       <c r="AU20" s="6"/>
       <c r="AV20" s="6"/>
       <c r="AW20" s="6"/>
@@ -1298,51 +1399,51 @@
     </row>
     <row r="21">
       <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="6"/>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="14"/>
+      <c r="AB21" s="14"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="14"/>
+      <c r="AE21" s="14"/>
       <c r="AF21" s="6"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="6"/>
       <c r="AK21" s="6"/>
-      <c r="AL21" s="11"/>
-      <c r="AM21" s="11"/>
-      <c r="AN21" s="11"/>
-      <c r="AO21" s="11"/>
-      <c r="AP21" s="11"/>
-      <c r="AQ21" s="11"/>
-      <c r="AR21" s="11"/>
-      <c r="AS21" s="11"/>
-      <c r="AT21" s="11"/>
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6"/>
+      <c r="AN21" s="6"/>
+      <c r="AO21" s="6"/>
+      <c r="AP21" s="6"/>
+      <c r="AQ21" s="6"/>
+      <c r="AR21" s="6"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="6"/>
       <c r="AU21" s="6"/>
       <c r="AV21" s="6"/>
       <c r="AW21" s="6"/>
@@ -1352,36 +1453,36 @@
     </row>
     <row r="22">
       <c r="A22" s="5"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="6"/>
-      <c r="AE22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="14"/>
+      <c r="X22" s="14"/>
+      <c r="Y22" s="14"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="14"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="14"/>
+      <c r="AE22" s="14"/>
       <c r="AF22" s="6"/>
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
@@ -1406,12 +1507,12 @@
     </row>
     <row r="23">
       <c r="A23" s="5"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="11"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -1460,12 +1561,12 @@
     </row>
     <row r="24">
       <c r="A24" s="8"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -1547,14 +1648,14 @@
       <c r="AF25" s="6"/>
       <c r="AG25" s="6"/>
       <c r="AH25" s="6"/>
-      <c r="AI25" s="11"/>
-      <c r="AJ25" s="11"/>
-      <c r="AK25" s="11"/>
-      <c r="AL25" s="11"/>
-      <c r="AM25" s="11"/>
-      <c r="AN25" s="11"/>
-      <c r="AO25" s="11"/>
-      <c r="AP25" s="11"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="6"/>
+      <c r="AK25" s="6"/>
+      <c r="AL25" s="6"/>
+      <c r="AM25" s="6"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="6"/>
+      <c r="AP25" s="6"/>
       <c r="AQ25" s="6"/>
       <c r="AR25" s="6"/>
       <c r="AS25" s="6"/>
@@ -1596,19 +1697,19 @@
       <c r="AA26" s="6"/>
       <c r="AB26" s="6"/>
       <c r="AC26" s="6"/>
-      <c r="AD26" s="6"/>
-      <c r="AE26" s="6"/>
-      <c r="AF26" s="6"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="15"/>
+      <c r="AF26" s="15"/>
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
-      <c r="AI26" s="11"/>
-      <c r="AJ26" s="13"/>
-      <c r="AK26" s="13"/>
-      <c r="AL26" s="13"/>
-      <c r="AM26" s="13"/>
-      <c r="AN26" s="13"/>
-      <c r="AO26" s="13"/>
-      <c r="AP26" s="11"/>
+      <c r="AI26" s="6"/>
+      <c r="AJ26" s="6"/>
+      <c r="AK26" s="6"/>
+      <c r="AL26" s="6"/>
+      <c r="AM26" s="6"/>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="6"/>
+      <c r="AP26" s="6"/>
       <c r="AQ26" s="6"/>
       <c r="AR26" s="6"/>
       <c r="AS26" s="6"/>
@@ -1629,40 +1730,40 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
       <c r="AA27" s="6"/>
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
-      <c r="AD27" s="6"/>
-      <c r="AE27" s="6"/>
-      <c r="AF27" s="6"/>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="15"/>
+      <c r="AF27" s="15"/>
       <c r="AG27" s="6"/>
       <c r="AH27" s="6"/>
-      <c r="AI27" s="11"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="11"/>
-      <c r="AL27" s="11"/>
-      <c r="AM27" s="11"/>
-      <c r="AN27" s="11"/>
-      <c r="AO27" s="11"/>
-      <c r="AP27" s="11"/>
+      <c r="AI27" s="6"/>
+      <c r="AJ27" s="6"/>
+      <c r="AK27" s="6"/>
+      <c r="AL27" s="6"/>
+      <c r="AM27" s="6"/>
+      <c r="AN27" s="6"/>
+      <c r="AO27" s="6"/>
+      <c r="AP27" s="6"/>
       <c r="AQ27" s="6"/>
       <c r="AR27" s="6"/>
       <c r="AS27" s="6"/>
@@ -1683,30 +1784,30 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="11"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
       <c r="AA28" s="6"/>
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
-      <c r="AD28" s="6"/>
-      <c r="AE28" s="6"/>
-      <c r="AF28" s="6"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="16"/>
+      <c r="AF28" s="16"/>
       <c r="AG28" s="6"/>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
@@ -1722,9 +1823,9 @@
       <c r="AS28" s="6"/>
       <c r="AT28" s="6"/>
       <c r="AU28" s="6"/>
-      <c r="AV28" s="11"/>
-      <c r="AW28" s="11"/>
-      <c r="AX28" s="14"/>
+      <c r="AV28" s="6"/>
+      <c r="AW28" s="6"/>
+      <c r="AX28" s="7"/>
       <c r="AY28" s="4"/>
       <c r="AZ28" s="4"/>
     </row>
@@ -1737,24 +1838,24 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6"/>
       <c r="AA29" s="6"/>
       <c r="AB29" s="6"/>
       <c r="AC29" s="6"/>
@@ -1776,9 +1877,9 @@
       <c r="AS29" s="6"/>
       <c r="AT29" s="6"/>
       <c r="AU29" s="6"/>
-      <c r="AV29" s="11"/>
-      <c r="AW29" s="13"/>
-      <c r="AX29" s="14"/>
+      <c r="AV29" s="6"/>
+      <c r="AW29" s="6"/>
+      <c r="AX29" s="7"/>
       <c r="AY29" s="4"/>
       <c r="AZ29" s="4"/>
     </row>
@@ -1830,18 +1931,18 @@
       <c r="AS30" s="9"/>
       <c r="AT30" s="9"/>
       <c r="AU30" s="9"/>
-      <c r="AV30" s="15"/>
-      <c r="AW30" s="15"/>
-      <c r="AX30" s="16"/>
+      <c r="AV30" s="9"/>
+      <c r="AW30" s="9"/>
+      <c r="AX30" s="10"/>
       <c r="AY30" s="4"/>
       <c r="AZ30" s="4"/>
     </row>
     <row r="31">
-      <c r="A31" s="12"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -1852,17 +1953,17 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
-      <c r="Y31" s="6"/>
-      <c r="Z31" s="6"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
       <c r="AA31" s="6"/>
       <c r="AB31" s="6"/>
       <c r="AC31" s="6"/>
@@ -1873,9 +1974,9 @@
       <c r="AH31" s="6"/>
       <c r="AI31" s="6"/>
       <c r="AJ31" s="6"/>
-      <c r="AK31" s="11"/>
-      <c r="AL31" s="11"/>
-      <c r="AM31" s="11"/>
+      <c r="AK31" s="6"/>
+      <c r="AL31" s="6"/>
+      <c r="AM31" s="6"/>
       <c r="AN31" s="6"/>
       <c r="AO31" s="6"/>
       <c r="AP31" s="6"/>
@@ -1891,34 +1992,34 @@
       <c r="AZ31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="11"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="6"/>
-      <c r="AB32" s="6"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="18"/>
+      <c r="AB32" s="18"/>
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
       <c r="AE32" s="6"/>
@@ -1927,17 +2028,17 @@
       <c r="AH32" s="6"/>
       <c r="AI32" s="6"/>
       <c r="AJ32" s="6"/>
-      <c r="AK32" s="11"/>
-      <c r="AL32" s="13"/>
-      <c r="AM32" s="11"/>
+      <c r="AK32" s="6"/>
+      <c r="AL32" s="6"/>
+      <c r="AM32" s="6"/>
       <c r="AN32" s="6"/>
       <c r="AO32" s="6"/>
       <c r="AP32" s="6"/>
       <c r="AQ32" s="6"/>
-      <c r="AR32" s="11"/>
-      <c r="AS32" s="11"/>
-      <c r="AT32" s="11"/>
-      <c r="AU32" s="11"/>
+      <c r="AR32" s="6"/>
+      <c r="AS32" s="6"/>
+      <c r="AT32" s="6"/>
+      <c r="AU32" s="6"/>
       <c r="AV32" s="6"/>
       <c r="AW32" s="6"/>
       <c r="AX32" s="7"/>
@@ -1945,34 +2046,34 @@
       <c r="AZ32" s="4"/>
     </row>
     <row r="33">
-      <c r="A33" s="12"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="6"/>
-      <c r="AB33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="19"/>
+      <c r="AA33" s="18"/>
+      <c r="AB33" s="18"/>
       <c r="AC33" s="6"/>
       <c r="AD33" s="6"/>
       <c r="AE33" s="6"/>
@@ -1981,17 +2082,17 @@
       <c r="AH33" s="6"/>
       <c r="AI33" s="6"/>
       <c r="AJ33" s="6"/>
-      <c r="AK33" s="11"/>
-      <c r="AL33" s="13"/>
-      <c r="AM33" s="11"/>
+      <c r="AK33" s="6"/>
+      <c r="AL33" s="6"/>
+      <c r="AM33" s="6"/>
       <c r="AN33" s="6"/>
       <c r="AO33" s="6"/>
       <c r="AP33" s="6"/>
       <c r="AQ33" s="6"/>
-      <c r="AR33" s="11"/>
-      <c r="AS33" s="13"/>
-      <c r="AT33" s="13"/>
-      <c r="AU33" s="11"/>
+      <c r="AR33" s="6"/>
+      <c r="AS33" s="6"/>
+      <c r="AT33" s="6"/>
+      <c r="AU33" s="6"/>
       <c r="AV33" s="6"/>
       <c r="AW33" s="6"/>
       <c r="AX33" s="7"/>
@@ -2009,24 +2110,24 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="11"/>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="11"/>
-      <c r="AA34" s="6"/>
-      <c r="AB34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="18"/>
+      <c r="AB34" s="18"/>
       <c r="AC34" s="6"/>
       <c r="AD34" s="6"/>
       <c r="AE34" s="6"/>
@@ -2035,17 +2136,17 @@
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
       <c r="AJ34" s="6"/>
-      <c r="AK34" s="11"/>
-      <c r="AL34" s="11"/>
-      <c r="AM34" s="11"/>
+      <c r="AK34" s="6"/>
+      <c r="AL34" s="6"/>
+      <c r="AM34" s="6"/>
       <c r="AN34" s="6"/>
       <c r="AO34" s="6"/>
       <c r="AP34" s="6"/>
       <c r="AQ34" s="6"/>
-      <c r="AR34" s="11"/>
-      <c r="AS34" s="11"/>
-      <c r="AT34" s="11"/>
-      <c r="AU34" s="11"/>
+      <c r="AR34" s="6"/>
+      <c r="AS34" s="6"/>
+      <c r="AT34" s="6"/>
+      <c r="AU34" s="6"/>
       <c r="AV34" s="6"/>
       <c r="AW34" s="6"/>
       <c r="AX34" s="7"/>
@@ -2063,9 +2164,9 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="11"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
@@ -2076,9 +2177,9 @@
       <c r="U35" s="6"/>
       <c r="V35" s="6"/>
       <c r="W35" s="6"/>
-      <c r="X35" s="11"/>
-      <c r="Y35" s="11"/>
-      <c r="Z35" s="11"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
       <c r="AA35" s="6"/>
       <c r="AB35" s="6"/>
       <c r="AC35" s="6"/>
@@ -2117,9 +2218,9 @@
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
@@ -2161,10 +2262,10 @@
       <c r="AZ36" s="4"/>
     </row>
     <row r="37">
-      <c r="A37" s="12"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
@@ -2195,30 +2296,30 @@
       <c r="AF37" s="6"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
-      <c r="AI37" s="11"/>
-      <c r="AJ37" s="11"/>
-      <c r="AK37" s="11"/>
-      <c r="AL37" s="11"/>
-      <c r="AM37" s="11"/>
-      <c r="AN37" s="11"/>
-      <c r="AO37" s="11"/>
-      <c r="AP37" s="11"/>
-      <c r="AQ37" s="11"/>
-      <c r="AR37" s="11"/>
-      <c r="AS37" s="11"/>
-      <c r="AT37" s="11"/>
-      <c r="AU37" s="11"/>
-      <c r="AV37" s="11"/>
-      <c r="AW37" s="11"/>
-      <c r="AX37" s="14"/>
+      <c r="AI37" s="6"/>
+      <c r="AJ37" s="6"/>
+      <c r="AK37" s="6"/>
+      <c r="AL37" s="6"/>
+      <c r="AM37" s="6"/>
+      <c r="AN37" s="6"/>
+      <c r="AO37" s="6"/>
+      <c r="AP37" s="6"/>
+      <c r="AQ37" s="6"/>
+      <c r="AR37" s="6"/>
+      <c r="AS37" s="6"/>
+      <c r="AT37" s="6"/>
+      <c r="AU37" s="6"/>
+      <c r="AV37" s="6"/>
+      <c r="AW37" s="6"/>
+      <c r="AX37" s="7"/>
       <c r="AY37" s="4"/>
       <c r="AZ37" s="4"/>
     </row>
     <row r="38">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="11"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
@@ -2227,9 +2328,9 @@
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
@@ -2241,38 +2342,38 @@
       <c r="X38" s="6"/>
       <c r="Y38" s="6"/>
       <c r="Z38" s="6"/>
-      <c r="AA38" s="6"/>
-      <c r="AB38" s="6"/>
-      <c r="AC38" s="6"/>
-      <c r="AD38" s="6"/>
-      <c r="AE38" s="6"/>
-      <c r="AF38" s="6"/>
-      <c r="AG38" s="6"/>
-      <c r="AH38" s="6"/>
-      <c r="AI38" s="11"/>
-      <c r="AJ38" s="13"/>
-      <c r="AK38" s="13"/>
-      <c r="AL38" s="13"/>
-      <c r="AM38" s="13"/>
-      <c r="AN38" s="13"/>
-      <c r="AO38" s="13"/>
-      <c r="AP38" s="13"/>
-      <c r="AQ38" s="13"/>
-      <c r="AR38" s="13"/>
-      <c r="AS38" s="13"/>
-      <c r="AT38" s="13"/>
-      <c r="AU38" s="13"/>
-      <c r="AV38" s="13"/>
-      <c r="AW38" s="13"/>
-      <c r="AX38" s="14"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="20"/>
+      <c r="AE38" s="20"/>
+      <c r="AF38" s="20"/>
+      <c r="AG38" s="20"/>
+      <c r="AH38" s="20"/>
+      <c r="AI38" s="20"/>
+      <c r="AJ38" s="20"/>
+      <c r="AK38" s="20"/>
+      <c r="AL38" s="6"/>
+      <c r="AM38" s="6"/>
+      <c r="AN38" s="6"/>
+      <c r="AO38" s="6"/>
+      <c r="AP38" s="6"/>
+      <c r="AQ38" s="6"/>
+      <c r="AR38" s="6"/>
+      <c r="AS38" s="6"/>
+      <c r="AT38" s="6"/>
+      <c r="AU38" s="6"/>
+      <c r="AV38" s="6"/>
+      <c r="AW38" s="6"/>
+      <c r="AX38" s="7"/>
       <c r="AY38" s="4"/>
       <c r="AZ38" s="4"/>
     </row>
     <row r="39">
-      <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
@@ -2281,9 +2382,9 @@
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
@@ -2295,30 +2396,30 @@
       <c r="X39" s="6"/>
       <c r="Y39" s="6"/>
       <c r="Z39" s="6"/>
-      <c r="AA39" s="6"/>
-      <c r="AB39" s="6"/>
-      <c r="AC39" s="6"/>
-      <c r="AD39" s="6"/>
-      <c r="AE39" s="6"/>
-      <c r="AF39" s="6"/>
-      <c r="AG39" s="6"/>
-      <c r="AH39" s="6"/>
-      <c r="AI39" s="11"/>
-      <c r="AJ39" s="11"/>
-      <c r="AK39" s="11"/>
-      <c r="AL39" s="11"/>
-      <c r="AM39" s="11"/>
-      <c r="AN39" s="11"/>
-      <c r="AO39" s="11"/>
-      <c r="AP39" s="11"/>
-      <c r="AQ39" s="11"/>
-      <c r="AR39" s="11"/>
-      <c r="AS39" s="11"/>
-      <c r="AT39" s="11"/>
-      <c r="AU39" s="11"/>
-      <c r="AV39" s="11"/>
-      <c r="AW39" s="11"/>
-      <c r="AX39" s="14"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="20"/>
+      <c r="AH39" s="20"/>
+      <c r="AI39" s="20"/>
+      <c r="AJ39" s="20"/>
+      <c r="AK39" s="20"/>
+      <c r="AL39" s="6"/>
+      <c r="AM39" s="6"/>
+      <c r="AN39" s="6"/>
+      <c r="AO39" s="6"/>
+      <c r="AP39" s="6"/>
+      <c r="AQ39" s="6"/>
+      <c r="AR39" s="6"/>
+      <c r="AS39" s="6"/>
+      <c r="AT39" s="6"/>
+      <c r="AU39" s="6"/>
+      <c r="AV39" s="6"/>
+      <c r="AW39" s="6"/>
+      <c r="AX39" s="7"/>
       <c r="AY39" s="4"/>
       <c r="AZ39" s="4"/>
     </row>
@@ -2335,31 +2436,31 @@
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
+      <c r="U40" s="6"/>
       <c r="V40" s="6"/>
       <c r="W40" s="6"/>
       <c r="X40" s="6"/>
       <c r="Y40" s="6"/>
       <c r="Z40" s="6"/>
-      <c r="AA40" s="6"/>
-      <c r="AB40" s="6"/>
-      <c r="AC40" s="6"/>
-      <c r="AD40" s="6"/>
-      <c r="AE40" s="6"/>
-      <c r="AF40" s="6"/>
-      <c r="AG40" s="6"/>
-      <c r="AH40" s="6"/>
-      <c r="AI40" s="6"/>
-      <c r="AJ40" s="6"/>
-      <c r="AK40" s="6"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="20"/>
+      <c r="AE40" s="20"/>
+      <c r="AF40" s="20"/>
+      <c r="AG40" s="20"/>
+      <c r="AH40" s="20"/>
+      <c r="AI40" s="20"/>
+      <c r="AJ40" s="20"/>
+      <c r="AK40" s="20"/>
       <c r="AL40" s="6"/>
       <c r="AM40" s="6"/>
       <c r="AN40" s="6"/>
@@ -2389,31 +2490,31 @@
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="11"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
       <c r="V41" s="6"/>
       <c r="W41" s="6"/>
       <c r="X41" s="6"/>
       <c r="Y41" s="6"/>
       <c r="Z41" s="6"/>
-      <c r="AA41" s="6"/>
-      <c r="AB41" s="6"/>
-      <c r="AC41" s="6"/>
-      <c r="AD41" s="6"/>
-      <c r="AE41" s="6"/>
-      <c r="AF41" s="6"/>
-      <c r="AG41" s="6"/>
-      <c r="AH41" s="6"/>
-      <c r="AI41" s="6"/>
-      <c r="AJ41" s="6"/>
-      <c r="AK41" s="6"/>
+      <c r="AA41" s="20"/>
+      <c r="AB41" s="20"/>
+      <c r="AC41" s="20"/>
+      <c r="AD41" s="20"/>
+      <c r="AE41" s="20"/>
+      <c r="AF41" s="20"/>
+      <c r="AG41" s="20"/>
+      <c r="AH41" s="20"/>
+      <c r="AI41" s="20"/>
+      <c r="AJ41" s="20"/>
+      <c r="AK41" s="20"/>
       <c r="AL41" s="6"/>
       <c r="AM41" s="6"/>
       <c r="AN41" s="6"/>
@@ -2443,15 +2544,15 @@
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="15"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
       <c r="V42" s="9"/>
       <c r="W42" s="9"/>
       <c r="X42" s="9"/>
@@ -2512,9 +2613,9 @@
       <c r="Y43" s="6"/>
       <c r="Z43" s="6"/>
       <c r="AA43" s="6"/>
-      <c r="AB43" s="11"/>
-      <c r="AC43" s="11"/>
-      <c r="AD43" s="11"/>
+      <c r="AB43" s="6"/>
+      <c r="AC43" s="6"/>
+      <c r="AD43" s="6"/>
       <c r="AE43" s="6"/>
       <c r="AF43" s="6"/>
       <c r="AG43" s="6"/>
@@ -2566,9 +2667,9 @@
       <c r="Y44" s="6"/>
       <c r="Z44" s="6"/>
       <c r="AA44" s="6"/>
-      <c r="AB44" s="11"/>
-      <c r="AC44" s="13"/>
-      <c r="AD44" s="11"/>
+      <c r="AB44" s="6"/>
+      <c r="AC44" s="6"/>
+      <c r="AD44" s="6"/>
       <c r="AE44" s="6"/>
       <c r="AF44" s="6"/>
       <c r="AG44" s="6"/>
@@ -2586,18 +2687,18 @@
       <c r="AS44" s="6"/>
       <c r="AT44" s="6"/>
       <c r="AU44" s="6"/>
-      <c r="AV44" s="6"/>
-      <c r="AW44" s="6"/>
-      <c r="AX44" s="7"/>
+      <c r="AV44" s="15"/>
+      <c r="AW44" s="15"/>
+      <c r="AX44" s="21"/>
       <c r="AY44" s="4"/>
       <c r="AZ44" s="4"/>
     </row>
     <row r="45">
-      <c r="A45" s="12"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
@@ -2607,9 +2708,9 @@
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
@@ -2620,38 +2721,38 @@
       <c r="Y45" s="6"/>
       <c r="Z45" s="6"/>
       <c r="AA45" s="6"/>
-      <c r="AB45" s="11"/>
-      <c r="AC45" s="13"/>
-      <c r="AD45" s="11"/>
-      <c r="AE45" s="6"/>
-      <c r="AF45" s="6"/>
-      <c r="AG45" s="6"/>
-      <c r="AH45" s="6"/>
-      <c r="AI45" s="6"/>
-      <c r="AJ45" s="6"/>
-      <c r="AK45" s="6"/>
+      <c r="AB45" s="6"/>
+      <c r="AC45" s="6"/>
+      <c r="AD45" s="6"/>
+      <c r="AE45" s="22"/>
+      <c r="AF45" s="22"/>
+      <c r="AG45" s="22"/>
+      <c r="AH45" s="22"/>
+      <c r="AI45" s="22"/>
+      <c r="AJ45" s="22"/>
+      <c r="AK45" s="22"/>
       <c r="AL45" s="6"/>
       <c r="AM45" s="6"/>
-      <c r="AN45" s="11"/>
-      <c r="AO45" s="11"/>
-      <c r="AP45" s="11"/>
+      <c r="AN45" s="6"/>
+      <c r="AO45" s="6"/>
+      <c r="AP45" s="6"/>
       <c r="AQ45" s="6"/>
       <c r="AR45" s="6"/>
       <c r="AS45" s="6"/>
       <c r="AT45" s="6"/>
       <c r="AU45" s="6"/>
-      <c r="AV45" s="6"/>
-      <c r="AW45" s="6"/>
-      <c r="AX45" s="7"/>
+      <c r="AV45" s="15"/>
+      <c r="AW45" s="15"/>
+      <c r="AX45" s="21"/>
       <c r="AY45" s="4"/>
       <c r="AZ45" s="4"/>
     </row>
     <row r="46">
-      <c r="A46" s="12"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="11"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -2661,9 +2762,9 @@
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="11"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
       <c r="S46" s="6"/>
       <c r="T46" s="6"/>
@@ -2674,38 +2775,38 @@
       <c r="Y46" s="6"/>
       <c r="Z46" s="6"/>
       <c r="AA46" s="6"/>
-      <c r="AB46" s="11"/>
-      <c r="AC46" s="11"/>
-      <c r="AD46" s="11"/>
-      <c r="AE46" s="6"/>
-      <c r="AF46" s="6"/>
-      <c r="AG46" s="6"/>
-      <c r="AH46" s="6"/>
-      <c r="AI46" s="6"/>
-      <c r="AJ46" s="6"/>
-      <c r="AK46" s="6"/>
+      <c r="AB46" s="6"/>
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6"/>
+      <c r="AE46" s="22"/>
+      <c r="AF46" s="22"/>
+      <c r="AG46" s="22"/>
+      <c r="AH46" s="22"/>
+      <c r="AI46" s="22"/>
+      <c r="AJ46" s="22"/>
+      <c r="AK46" s="22"/>
       <c r="AL46" s="6"/>
       <c r="AM46" s="6"/>
-      <c r="AN46" s="11"/>
-      <c r="AO46" s="13"/>
-      <c r="AP46" s="11"/>
+      <c r="AN46" s="6"/>
+      <c r="AO46" s="6"/>
+      <c r="AP46" s="6"/>
       <c r="AQ46" s="6"/>
       <c r="AR46" s="6"/>
       <c r="AS46" s="6"/>
       <c r="AT46" s="6"/>
       <c r="AU46" s="6"/>
-      <c r="AV46" s="6"/>
-      <c r="AW46" s="6"/>
-      <c r="AX46" s="7"/>
+      <c r="AV46" s="15"/>
+      <c r="AW46" s="15"/>
+      <c r="AX46" s="21"/>
       <c r="AY46" s="4"/>
       <c r="AZ46" s="4"/>
     </row>
     <row r="47">
-      <c r="A47" s="12"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
@@ -2715,9 +2816,9 @@
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="11"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
@@ -2740,9 +2841,9 @@
       <c r="AK47" s="6"/>
       <c r="AL47" s="6"/>
       <c r="AM47" s="6"/>
-      <c r="AN47" s="11"/>
-      <c r="AO47" s="13"/>
-      <c r="AP47" s="11"/>
+      <c r="AN47" s="6"/>
+      <c r="AO47" s="6"/>
+      <c r="AP47" s="6"/>
       <c r="AQ47" s="6"/>
       <c r="AR47" s="6"/>
       <c r="AS47" s="6"/>
@@ -2769,9 +2870,9 @@
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
       <c r="R48" s="9"/>
       <c r="S48" s="9"/>
       <c r="T48" s="9"/>
@@ -2794,9 +2895,9 @@
       <c r="AK48" s="9"/>
       <c r="AL48" s="9"/>
       <c r="AM48" s="9"/>
-      <c r="AN48" s="15"/>
-      <c r="AO48" s="15"/>
-      <c r="AP48" s="15"/>
+      <c r="AN48" s="9"/>
+      <c r="AO48" s="9"/>
+      <c r="AP48" s="9"/>
       <c r="AQ48" s="9"/>
       <c r="AR48" s="9"/>
       <c r="AS48" s="9"/>
@@ -2870,49 +2971,49 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="6"/>
-      <c r="S50" s="6"/>
-      <c r="T50" s="6"/>
-      <c r="U50" s="6"/>
-      <c r="V50" s="6"/>
-      <c r="W50" s="11"/>
-      <c r="X50" s="11"/>
-      <c r="Y50" s="11"/>
-      <c r="Z50" s="11"/>
-      <c r="AA50" s="11"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="23"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="23"/>
+      <c r="T50" s="23"/>
+      <c r="U50" s="23"/>
+      <c r="V50" s="23"/>
+      <c r="W50" s="23"/>
+      <c r="X50" s="23"/>
+      <c r="Y50" s="23"/>
+      <c r="Z50" s="23"/>
+      <c r="AA50" s="23"/>
       <c r="AB50" s="6"/>
       <c r="AC50" s="6"/>
       <c r="AD50" s="6"/>
       <c r="AE50" s="6"/>
       <c r="AF50" s="6"/>
-      <c r="AG50" s="11"/>
-      <c r="AH50" s="11"/>
-      <c r="AI50" s="11"/>
-      <c r="AJ50" s="11"/>
-      <c r="AK50" s="11"/>
-      <c r="AL50" s="11"/>
-      <c r="AM50" s="11"/>
-      <c r="AN50" s="11"/>
-      <c r="AO50" s="11"/>
-      <c r="AP50" s="11"/>
-      <c r="AQ50" s="11"/>
+      <c r="AG50" s="6"/>
+      <c r="AH50" s="6"/>
+      <c r="AI50" s="6"/>
+      <c r="AJ50" s="6"/>
+      <c r="AK50" s="6"/>
+      <c r="AL50" s="6"/>
+      <c r="AM50" s="6"/>
+      <c r="AN50" s="6"/>
+      <c r="AO50" s="6"/>
+      <c r="AP50" s="6"/>
+      <c r="AQ50" s="6"/>
       <c r="AR50" s="6"/>
       <c r="AS50" s="6"/>
       <c r="AT50" s="6"/>
       <c r="AU50" s="6"/>
-      <c r="AV50" s="6"/>
-      <c r="AW50" s="6"/>
-      <c r="AX50" s="7"/>
+      <c r="AV50" s="15"/>
+      <c r="AW50" s="15"/>
+      <c r="AX50" s="21"/>
       <c r="AY50" s="4"/>
       <c r="AZ50" s="4"/>
     </row>
@@ -2924,49 +3025,49 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="13"/>
-      <c r="P51" s="13"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="6"/>
-      <c r="U51" s="6"/>
-      <c r="V51" s="6"/>
-      <c r="W51" s="11"/>
-      <c r="X51" s="13"/>
-      <c r="Y51" s="13"/>
-      <c r="Z51" s="13"/>
-      <c r="AA51" s="11"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="23"/>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="23"/>
+      <c r="S51" s="23"/>
+      <c r="T51" s="23"/>
+      <c r="U51" s="23"/>
+      <c r="V51" s="23"/>
+      <c r="W51" s="23"/>
+      <c r="X51" s="23"/>
+      <c r="Y51" s="23"/>
+      <c r="Z51" s="23"/>
+      <c r="AA51" s="23"/>
       <c r="AB51" s="6"/>
       <c r="AC51" s="6"/>
       <c r="AD51" s="6"/>
       <c r="AE51" s="6"/>
       <c r="AF51" s="6"/>
-      <c r="AG51" s="11"/>
-      <c r="AH51" s="13"/>
-      <c r="AI51" s="13"/>
-      <c r="AJ51" s="13"/>
-      <c r="AK51" s="13"/>
-      <c r="AL51" s="13"/>
-      <c r="AM51" s="13"/>
-      <c r="AN51" s="13"/>
-      <c r="AO51" s="13"/>
-      <c r="AP51" s="13"/>
-      <c r="AQ51" s="11"/>
+      <c r="AG51" s="6"/>
+      <c r="AH51" s="6"/>
+      <c r="AI51" s="6"/>
+      <c r="AJ51" s="6"/>
+      <c r="AK51" s="6"/>
+      <c r="AL51" s="6"/>
+      <c r="AM51" s="6"/>
+      <c r="AN51" s="6"/>
+      <c r="AO51" s="6"/>
+      <c r="AP51" s="6"/>
+      <c r="AQ51" s="6"/>
       <c r="AR51" s="6"/>
       <c r="AS51" s="6"/>
       <c r="AT51" s="6"/>
       <c r="AU51" s="6"/>
-      <c r="AV51" s="6"/>
-      <c r="AW51" s="6"/>
-      <c r="AX51" s="7"/>
+      <c r="AV51" s="15"/>
+      <c r="AW51" s="15"/>
+      <c r="AX51" s="21"/>
       <c r="AY51" s="4"/>
       <c r="AZ51" s="4"/>
     </row>
@@ -2978,49 +3079,49 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="6"/>
-      <c r="S52" s="6"/>
-      <c r="T52" s="6"/>
-      <c r="U52" s="6"/>
-      <c r="V52" s="6"/>
-      <c r="W52" s="11"/>
-      <c r="X52" s="11"/>
-      <c r="Y52" s="11"/>
-      <c r="Z52" s="11"/>
-      <c r="AA52" s="11"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="23"/>
+      <c r="L52" s="23"/>
+      <c r="M52" s="23"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="23"/>
+      <c r="P52" s="23"/>
+      <c r="Q52" s="23"/>
+      <c r="R52" s="23"/>
+      <c r="S52" s="23"/>
+      <c r="T52" s="23"/>
+      <c r="U52" s="23"/>
+      <c r="V52" s="23"/>
+      <c r="W52" s="23"/>
+      <c r="X52" s="23"/>
+      <c r="Y52" s="23"/>
+      <c r="Z52" s="23"/>
+      <c r="AA52" s="23"/>
       <c r="AB52" s="6"/>
       <c r="AC52" s="6"/>
       <c r="AD52" s="6"/>
       <c r="AE52" s="6"/>
       <c r="AF52" s="6"/>
-      <c r="AG52" s="11"/>
-      <c r="AH52" s="11"/>
-      <c r="AI52" s="11"/>
-      <c r="AJ52" s="11"/>
-      <c r="AK52" s="11"/>
-      <c r="AL52" s="11"/>
-      <c r="AM52" s="11"/>
-      <c r="AN52" s="11"/>
-      <c r="AO52" s="11"/>
-      <c r="AP52" s="11"/>
-      <c r="AQ52" s="11"/>
+      <c r="AG52" s="6"/>
+      <c r="AH52" s="6"/>
+      <c r="AI52" s="6"/>
+      <c r="AJ52" s="6"/>
+      <c r="AK52" s="6"/>
+      <c r="AL52" s="6"/>
+      <c r="AM52" s="6"/>
+      <c r="AN52" s="6"/>
+      <c r="AO52" s="6"/>
+      <c r="AP52" s="6"/>
+      <c r="AQ52" s="6"/>
       <c r="AR52" s="6"/>
       <c r="AS52" s="6"/>
       <c r="AT52" s="6"/>
       <c r="AU52" s="6"/>
-      <c r="AV52" s="6"/>
-      <c r="AW52" s="6"/>
-      <c r="AX52" s="7"/>
+      <c r="AV52" s="15"/>
+      <c r="AW52" s="15"/>
+      <c r="AX52" s="21"/>
       <c r="AY52" s="4"/>
       <c r="AZ52" s="4"/>
     </row>
@@ -3220,32 +3321,32 @@
       <c r="AE56" s="6"/>
       <c r="AF56" s="6"/>
       <c r="AG56" s="6"/>
-      <c r="AH56" s="6"/>
-      <c r="AI56" s="6"/>
-      <c r="AJ56" s="6"/>
-      <c r="AK56" s="6"/>
-      <c r="AL56" s="6"/>
-      <c r="AM56" s="6"/>
-      <c r="AN56" s="6"/>
-      <c r="AO56" s="6"/>
-      <c r="AP56" s="6"/>
-      <c r="AQ56" s="6"/>
+      <c r="AH56" s="24"/>
+      <c r="AI56" s="24"/>
+      <c r="AJ56" s="24"/>
+      <c r="AK56" s="24"/>
+      <c r="AL56" s="24"/>
+      <c r="AM56" s="24"/>
+      <c r="AN56" s="24"/>
+      <c r="AO56" s="24"/>
+      <c r="AP56" s="24"/>
+      <c r="AQ56" s="24"/>
       <c r="AR56" s="6"/>
       <c r="AS56" s="6"/>
-      <c r="AT56" s="11"/>
-      <c r="AU56" s="11"/>
-      <c r="AV56" s="11"/>
-      <c r="AW56" s="11"/>
-      <c r="AX56" s="14"/>
+      <c r="AT56" s="6"/>
+      <c r="AU56" s="6"/>
+      <c r="AV56" s="15"/>
+      <c r="AW56" s="15"/>
+      <c r="AX56" s="21"/>
       <c r="AY56" s="4"/>
       <c r="AZ56" s="4"/>
     </row>
     <row r="57">
-      <c r="A57" s="12"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
@@ -3258,48 +3359,48 @@
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
       <c r="Q57" s="6"/>
-      <c r="R57" s="11"/>
-      <c r="S57" s="11"/>
-      <c r="T57" s="11"/>
-      <c r="U57" s="11"/>
-      <c r="V57" s="11"/>
-      <c r="W57" s="11"/>
-      <c r="X57" s="11"/>
-      <c r="Y57" s="11"/>
-      <c r="Z57" s="11"/>
-      <c r="AA57" s="11"/>
-      <c r="AB57" s="11"/>
-      <c r="AC57" s="11"/>
-      <c r="AD57" s="11"/>
-      <c r="AE57" s="11"/>
-      <c r="AF57" s="11"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+      <c r="U57" s="6"/>
+      <c r="V57" s="6"/>
+      <c r="W57" s="6"/>
+      <c r="X57" s="6"/>
+      <c r="Y57" s="6"/>
+      <c r="Z57" s="6"/>
+      <c r="AA57" s="6"/>
+      <c r="AB57" s="6"/>
+      <c r="AC57" s="6"/>
+      <c r="AD57" s="6"/>
+      <c r="AE57" s="6"/>
+      <c r="AF57" s="6"/>
       <c r="AG57" s="6"/>
-      <c r="AH57" s="6"/>
-      <c r="AI57" s="6"/>
-      <c r="AJ57" s="6"/>
-      <c r="AK57" s="6"/>
-      <c r="AL57" s="6"/>
-      <c r="AM57" s="6"/>
-      <c r="AN57" s="6"/>
-      <c r="AO57" s="6"/>
-      <c r="AP57" s="6"/>
-      <c r="AQ57" s="6"/>
+      <c r="AH57" s="24"/>
+      <c r="AI57" s="24"/>
+      <c r="AJ57" s="24"/>
+      <c r="AK57" s="24"/>
+      <c r="AL57" s="24"/>
+      <c r="AM57" s="24"/>
+      <c r="AN57" s="24"/>
+      <c r="AO57" s="24"/>
+      <c r="AP57" s="24"/>
+      <c r="AQ57" s="24"/>
       <c r="AR57" s="6"/>
       <c r="AS57" s="6"/>
-      <c r="AT57" s="11"/>
-      <c r="AU57" s="13"/>
-      <c r="AV57" s="13"/>
-      <c r="AW57" s="13"/>
-      <c r="AX57" s="14"/>
+      <c r="AT57" s="6"/>
+      <c r="AU57" s="6"/>
+      <c r="AV57" s="15"/>
+      <c r="AW57" s="15"/>
+      <c r="AX57" s="21"/>
       <c r="AY57" s="4"/>
       <c r="AZ57" s="4"/>
     </row>
     <row r="58">
-      <c r="A58" s="12"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="11"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
@@ -3312,48 +3413,48 @@
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="13"/>
-      <c r="T58" s="13"/>
-      <c r="U58" s="13"/>
-      <c r="V58" s="13"/>
-      <c r="W58" s="13"/>
-      <c r="X58" s="13"/>
-      <c r="Y58" s="13"/>
-      <c r="Z58" s="13"/>
-      <c r="AA58" s="13"/>
-      <c r="AB58" s="13"/>
-      <c r="AC58" s="13"/>
-      <c r="AD58" s="13"/>
-      <c r="AE58" s="13"/>
-      <c r="AF58" s="11"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+      <c r="W58" s="6"/>
+      <c r="X58" s="6"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="6"/>
+      <c r="AA58" s="6"/>
+      <c r="AB58" s="6"/>
+      <c r="AC58" s="6"/>
+      <c r="AD58" s="6"/>
+      <c r="AE58" s="6"/>
+      <c r="AF58" s="6"/>
       <c r="AG58" s="6"/>
-      <c r="AH58" s="6"/>
-      <c r="AI58" s="6"/>
-      <c r="AJ58" s="6"/>
-      <c r="AK58" s="6"/>
-      <c r="AL58" s="6"/>
-      <c r="AM58" s="6"/>
-      <c r="AN58" s="6"/>
-      <c r="AO58" s="6"/>
-      <c r="AP58" s="6"/>
-      <c r="AQ58" s="6"/>
+      <c r="AH58" s="24"/>
+      <c r="AI58" s="24"/>
+      <c r="AJ58" s="24"/>
+      <c r="AK58" s="24"/>
+      <c r="AL58" s="24"/>
+      <c r="AM58" s="24"/>
+      <c r="AN58" s="24"/>
+      <c r="AO58" s="24"/>
+      <c r="AP58" s="24"/>
+      <c r="AQ58" s="24"/>
       <c r="AR58" s="6"/>
       <c r="AS58" s="6"/>
-      <c r="AT58" s="11"/>
-      <c r="AU58" s="11"/>
-      <c r="AV58" s="11"/>
-      <c r="AW58" s="11"/>
-      <c r="AX58" s="14"/>
+      <c r="AT58" s="6"/>
+      <c r="AU58" s="6"/>
+      <c r="AV58" s="15"/>
+      <c r="AW58" s="15"/>
+      <c r="AX58" s="21"/>
       <c r="AY58" s="4"/>
       <c r="AZ58" s="4"/>
     </row>
     <row r="59">
-      <c r="A59" s="12"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
@@ -3366,21 +3467,21 @@
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
       <c r="Q59" s="6"/>
-      <c r="R59" s="11"/>
-      <c r="S59" s="11"/>
-      <c r="T59" s="11"/>
-      <c r="U59" s="11"/>
-      <c r="V59" s="11"/>
-      <c r="W59" s="11"/>
-      <c r="X59" s="11"/>
-      <c r="Y59" s="11"/>
-      <c r="Z59" s="11"/>
-      <c r="AA59" s="11"/>
-      <c r="AB59" s="11"/>
-      <c r="AC59" s="11"/>
-      <c r="AD59" s="11"/>
-      <c r="AE59" s="11"/>
-      <c r="AF59" s="11"/>
+      <c r="R59" s="6"/>
+      <c r="S59" s="6"/>
+      <c r="T59" s="6"/>
+      <c r="U59" s="6"/>
+      <c r="V59" s="6"/>
+      <c r="W59" s="6"/>
+      <c r="X59" s="6"/>
+      <c r="Y59" s="6"/>
+      <c r="Z59" s="6"/>
+      <c r="AA59" s="6"/>
+      <c r="AB59" s="6"/>
+      <c r="AC59" s="6"/>
+      <c r="AD59" s="6"/>
+      <c r="AE59" s="6"/>
+      <c r="AF59" s="6"/>
       <c r="AG59" s="6"/>
       <c r="AH59" s="6"/>
       <c r="AI59" s="6"/>
@@ -3511,164 +3612,164 @@
       <c r="AZ61" s="4"/>
     </row>
     <row r="62">
-      <c r="A62" s="12"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="11"/>
-      <c r="N62" s="11"/>
-      <c r="O62" s="6"/>
-      <c r="P62" s="6"/>
-      <c r="Q62" s="6"/>
-      <c r="R62" s="6"/>
-      <c r="S62" s="6"/>
-      <c r="T62" s="11"/>
-      <c r="U62" s="11"/>
-      <c r="V62" s="11"/>
-      <c r="W62" s="11"/>
-      <c r="X62" s="11"/>
-      <c r="Y62" s="11"/>
-      <c r="Z62" s="11"/>
-      <c r="AA62" s="11"/>
-      <c r="AB62" s="11"/>
-      <c r="AC62" s="11"/>
-      <c r="AD62" s="11"/>
-      <c r="AE62" s="11"/>
-      <c r="AF62" s="11"/>
-      <c r="AG62" s="11"/>
-      <c r="AH62" s="11"/>
-      <c r="AI62" s="11"/>
-      <c r="AJ62" s="6"/>
-      <c r="AK62" s="6"/>
-      <c r="AL62" s="6"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="25"/>
+      <c r="J62" s="25"/>
+      <c r="K62" s="25"/>
+      <c r="L62" s="25"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="25"/>
+      <c r="O62" s="25"/>
+      <c r="P62" s="25"/>
+      <c r="Q62" s="25"/>
+      <c r="R62" s="25"/>
+      <c r="S62" s="25"/>
+      <c r="T62" s="25"/>
+      <c r="U62" s="25"/>
+      <c r="V62" s="25"/>
+      <c r="W62" s="25"/>
+      <c r="X62" s="25"/>
+      <c r="Y62" s="25"/>
+      <c r="Z62" s="25"/>
+      <c r="AA62" s="25"/>
+      <c r="AB62" s="25"/>
+      <c r="AC62" s="25"/>
+      <c r="AD62" s="25"/>
+      <c r="AE62" s="25"/>
+      <c r="AF62" s="25"/>
+      <c r="AG62" s="25"/>
+      <c r="AH62" s="25"/>
+      <c r="AI62" s="25"/>
+      <c r="AJ62" s="25"/>
+      <c r="AK62" s="25"/>
+      <c r="AL62" s="25"/>
       <c r="AM62" s="6"/>
       <c r="AN62" s="6"/>
       <c r="AO62" s="6"/>
-      <c r="AP62" s="11"/>
-      <c r="AQ62" s="11"/>
-      <c r="AR62" s="11"/>
-      <c r="AS62" s="11"/>
-      <c r="AT62" s="11"/>
-      <c r="AU62" s="11"/>
-      <c r="AV62" s="11"/>
-      <c r="AW62" s="11"/>
-      <c r="AX62" s="14"/>
+      <c r="AP62" s="6"/>
+      <c r="AQ62" s="6"/>
+      <c r="AR62" s="6"/>
+      <c r="AS62" s="6"/>
+      <c r="AT62" s="6"/>
+      <c r="AU62" s="6"/>
+      <c r="AV62" s="6"/>
+      <c r="AW62" s="6"/>
+      <c r="AX62" s="7"/>
       <c r="AY62" s="4"/>
       <c r="AZ62" s="4"/>
     </row>
     <row r="63">
-      <c r="A63" s="12"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="11"/>
-      <c r="O63" s="6"/>
-      <c r="P63" s="6"/>
-      <c r="Q63" s="6"/>
-      <c r="R63" s="6"/>
-      <c r="S63" s="6"/>
-      <c r="T63" s="11"/>
-      <c r="U63" s="13"/>
-      <c r="V63" s="13"/>
-      <c r="W63" s="13"/>
-      <c r="X63" s="13"/>
-      <c r="Y63" s="13"/>
-      <c r="Z63" s="13"/>
-      <c r="AA63" s="13"/>
-      <c r="AB63" s="13"/>
-      <c r="AC63" s="13"/>
-      <c r="AD63" s="13"/>
-      <c r="AE63" s="13"/>
-      <c r="AF63" s="13"/>
-      <c r="AG63" s="13"/>
-      <c r="AH63" s="13"/>
-      <c r="AI63" s="11"/>
-      <c r="AJ63" s="6"/>
-      <c r="AK63" s="6"/>
-      <c r="AL63" s="6"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="25"/>
+      <c r="J63" s="25"/>
+      <c r="K63" s="25"/>
+      <c r="L63" s="25"/>
+      <c r="M63" s="25"/>
+      <c r="N63" s="25"/>
+      <c r="O63" s="25"/>
+      <c r="P63" s="25"/>
+      <c r="Q63" s="25"/>
+      <c r="R63" s="25"/>
+      <c r="S63" s="25"/>
+      <c r="T63" s="25"/>
+      <c r="U63" s="25"/>
+      <c r="V63" s="25"/>
+      <c r="W63" s="25"/>
+      <c r="X63" s="25"/>
+      <c r="Y63" s="25"/>
+      <c r="Z63" s="25"/>
+      <c r="AA63" s="25"/>
+      <c r="AB63" s="25"/>
+      <c r="AC63" s="25"/>
+      <c r="AD63" s="25"/>
+      <c r="AE63" s="25"/>
+      <c r="AF63" s="25"/>
+      <c r="AG63" s="25"/>
+      <c r="AH63" s="25"/>
+      <c r="AI63" s="25"/>
+      <c r="AJ63" s="25"/>
+      <c r="AK63" s="25"/>
+      <c r="AL63" s="25"/>
       <c r="AM63" s="6"/>
       <c r="AN63" s="6"/>
       <c r="AO63" s="6"/>
-      <c r="AP63" s="11"/>
-      <c r="AQ63" s="13"/>
-      <c r="AR63" s="13"/>
-      <c r="AS63" s="13"/>
-      <c r="AT63" s="13"/>
-      <c r="AU63" s="13"/>
-      <c r="AV63" s="13"/>
-      <c r="AW63" s="13"/>
-      <c r="AX63" s="14"/>
+      <c r="AP63" s="6"/>
+      <c r="AQ63" s="6"/>
+      <c r="AR63" s="6"/>
+      <c r="AS63" s="6"/>
+      <c r="AT63" s="6"/>
+      <c r="AU63" s="6"/>
+      <c r="AV63" s="6"/>
+      <c r="AW63" s="6"/>
+      <c r="AX63" s="7"/>
       <c r="AY63" s="4"/>
       <c r="AZ63" s="4"/>
     </row>
     <row r="64">
-      <c r="A64" s="12"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-      <c r="N64" s="11"/>
-      <c r="O64" s="6"/>
-      <c r="P64" s="6"/>
-      <c r="Q64" s="6"/>
-      <c r="R64" s="6"/>
-      <c r="S64" s="6"/>
-      <c r="T64" s="11"/>
-      <c r="U64" s="11"/>
-      <c r="V64" s="11"/>
-      <c r="W64" s="11"/>
-      <c r="X64" s="11"/>
-      <c r="Y64" s="11"/>
-      <c r="Z64" s="11"/>
-      <c r="AA64" s="11"/>
-      <c r="AB64" s="11"/>
-      <c r="AC64" s="11"/>
-      <c r="AD64" s="11"/>
-      <c r="AE64" s="11"/>
-      <c r="AF64" s="11"/>
-      <c r="AG64" s="11"/>
-      <c r="AH64" s="11"/>
-      <c r="AI64" s="11"/>
-      <c r="AJ64" s="6"/>
-      <c r="AK64" s="6"/>
-      <c r="AL64" s="6"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="25"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="25"/>
+      <c r="O64" s="25"/>
+      <c r="P64" s="25"/>
+      <c r="Q64" s="25"/>
+      <c r="R64" s="25"/>
+      <c r="S64" s="25"/>
+      <c r="T64" s="25"/>
+      <c r="U64" s="25"/>
+      <c r="V64" s="25"/>
+      <c r="W64" s="25"/>
+      <c r="X64" s="25"/>
+      <c r="Y64" s="25"/>
+      <c r="Z64" s="25"/>
+      <c r="AA64" s="25"/>
+      <c r="AB64" s="25"/>
+      <c r="AC64" s="25"/>
+      <c r="AD64" s="25"/>
+      <c r="AE64" s="25"/>
+      <c r="AF64" s="25"/>
+      <c r="AG64" s="25"/>
+      <c r="AH64" s="25"/>
+      <c r="AI64" s="25"/>
+      <c r="AJ64" s="25"/>
+      <c r="AK64" s="25"/>
+      <c r="AL64" s="25"/>
       <c r="AM64" s="6"/>
       <c r="AN64" s="6"/>
       <c r="AO64" s="6"/>
-      <c r="AP64" s="11"/>
-      <c r="AQ64" s="11"/>
-      <c r="AR64" s="11"/>
-      <c r="AS64" s="11"/>
-      <c r="AT64" s="11"/>
-      <c r="AU64" s="11"/>
-      <c r="AV64" s="11"/>
-      <c r="AW64" s="11"/>
-      <c r="AX64" s="14"/>
+      <c r="AP64" s="6"/>
+      <c r="AQ64" s="6"/>
+      <c r="AR64" s="6"/>
+      <c r="AS64" s="6"/>
+      <c r="AT64" s="6"/>
+      <c r="AU64" s="6"/>
+      <c r="AV64" s="6"/>
+      <c r="AW64" s="6"/>
+      <c r="AX64" s="7"/>
       <c r="AY64" s="4"/>
       <c r="AZ64" s="4"/>
     </row>
@@ -3889,50 +3990,50 @@
       <c r="AZ68" s="4"/>
     </row>
     <row r="69">
-      <c r="A69" s="12"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="11"/>
-      <c r="T69" s="11"/>
-      <c r="U69" s="11"/>
-      <c r="V69" s="11"/>
-      <c r="W69" s="11"/>
-      <c r="X69" s="11"/>
-      <c r="Y69" s="11"/>
-      <c r="Z69" s="6"/>
-      <c r="AA69" s="6"/>
-      <c r="AB69" s="6"/>
-      <c r="AC69" s="6"/>
-      <c r="AD69" s="6"/>
-      <c r="AE69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="6"/>
+      <c r="T69" s="6"/>
+      <c r="U69" s="26"/>
+      <c r="V69" s="26"/>
+      <c r="W69" s="26"/>
+      <c r="X69" s="26"/>
+      <c r="Y69" s="26"/>
+      <c r="Z69" s="26"/>
+      <c r="AA69" s="26"/>
+      <c r="AB69" s="26"/>
+      <c r="AC69" s="26"/>
+      <c r="AD69" s="26"/>
+      <c r="AE69" s="26"/>
       <c r="AF69" s="6"/>
       <c r="AG69" s="6"/>
       <c r="AH69" s="6"/>
-      <c r="AI69" s="11"/>
-      <c r="AJ69" s="11"/>
-      <c r="AK69" s="11"/>
-      <c r="AL69" s="11"/>
-      <c r="AM69" s="11"/>
-      <c r="AN69" s="11"/>
-      <c r="AO69" s="11"/>
-      <c r="AP69" s="11"/>
-      <c r="AQ69" s="11"/>
-      <c r="AR69" s="11"/>
+      <c r="AI69" s="6"/>
+      <c r="AJ69" s="6"/>
+      <c r="AK69" s="6"/>
+      <c r="AL69" s="6"/>
+      <c r="AM69" s="6"/>
+      <c r="AN69" s="6"/>
+      <c r="AO69" s="6"/>
+      <c r="AP69" s="6"/>
+      <c r="AQ69" s="6"/>
+      <c r="AR69" s="6"/>
       <c r="AS69" s="6"/>
       <c r="AT69" s="6"/>
       <c r="AU69" s="6"/>
@@ -3943,50 +4044,50 @@
       <c r="AZ69" s="4"/>
     </row>
     <row r="70">
-      <c r="A70" s="12"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="11"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="13"/>
-      <c r="N70" s="13"/>
-      <c r="O70" s="13"/>
-      <c r="P70" s="13"/>
-      <c r="Q70" s="13"/>
-      <c r="R70" s="13"/>
-      <c r="S70" s="13"/>
-      <c r="T70" s="13"/>
-      <c r="U70" s="13"/>
-      <c r="V70" s="13"/>
-      <c r="W70" s="13"/>
-      <c r="X70" s="13"/>
-      <c r="Y70" s="11"/>
-      <c r="Z70" s="6"/>
-      <c r="AA70" s="6"/>
-      <c r="AB70" s="6"/>
-      <c r="AC70" s="6"/>
-      <c r="AD70" s="6"/>
-      <c r="AE70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="6"/>
+      <c r="T70" s="6"/>
+      <c r="U70" s="26"/>
+      <c r="V70" s="26"/>
+      <c r="W70" s="26"/>
+      <c r="X70" s="26"/>
+      <c r="Y70" s="26"/>
+      <c r="Z70" s="26"/>
+      <c r="AA70" s="26"/>
+      <c r="AB70" s="26"/>
+      <c r="AC70" s="26"/>
+      <c r="AD70" s="26"/>
+      <c r="AE70" s="26"/>
       <c r="AF70" s="6"/>
       <c r="AG70" s="6"/>
       <c r="AH70" s="6"/>
-      <c r="AI70" s="11"/>
-      <c r="AJ70" s="13"/>
-      <c r="AK70" s="13"/>
-      <c r="AL70" s="13"/>
-      <c r="AM70" s="13"/>
-      <c r="AN70" s="13"/>
-      <c r="AO70" s="13"/>
-      <c r="AP70" s="13"/>
-      <c r="AQ70" s="13"/>
-      <c r="AR70" s="11"/>
+      <c r="AI70" s="6"/>
+      <c r="AJ70" s="6"/>
+      <c r="AK70" s="6"/>
+      <c r="AL70" s="6"/>
+      <c r="AM70" s="6"/>
+      <c r="AN70" s="6"/>
+      <c r="AO70" s="6"/>
+      <c r="AP70" s="6"/>
+      <c r="AQ70" s="6"/>
+      <c r="AR70" s="6"/>
       <c r="AS70" s="6"/>
       <c r="AT70" s="6"/>
       <c r="AU70" s="6"/>
@@ -3997,31 +4098,31 @@
       <c r="AZ70" s="4"/>
     </row>
     <row r="71">
-      <c r="A71" s="12"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="11"/>
-      <c r="O71" s="11"/>
-      <c r="P71" s="11"/>
-      <c r="Q71" s="11"/>
-      <c r="R71" s="11"/>
-      <c r="S71" s="11"/>
-      <c r="T71" s="11"/>
-      <c r="U71" s="11"/>
-      <c r="V71" s="11"/>
-      <c r="W71" s="11"/>
-      <c r="X71" s="11"/>
-      <c r="Y71" s="11"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
+      <c r="Q71" s="6"/>
+      <c r="R71" s="6"/>
+      <c r="S71" s="6"/>
+      <c r="T71" s="6"/>
+      <c r="U71" s="6"/>
+      <c r="V71" s="6"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="6"/>
+      <c r="Y71" s="6"/>
       <c r="Z71" s="6"/>
       <c r="AA71" s="6"/>
       <c r="AB71" s="6"/>
@@ -4031,16 +4132,16 @@
       <c r="AF71" s="6"/>
       <c r="AG71" s="6"/>
       <c r="AH71" s="6"/>
-      <c r="AI71" s="11"/>
-      <c r="AJ71" s="11"/>
-      <c r="AK71" s="11"/>
-      <c r="AL71" s="11"/>
-      <c r="AM71" s="11"/>
-      <c r="AN71" s="11"/>
-      <c r="AO71" s="11"/>
-      <c r="AP71" s="11"/>
-      <c r="AQ71" s="11"/>
-      <c r="AR71" s="11"/>
+      <c r="AI71" s="6"/>
+      <c r="AJ71" s="6"/>
+      <c r="AK71" s="6"/>
+      <c r="AL71" s="6"/>
+      <c r="AM71" s="6"/>
+      <c r="AN71" s="6"/>
+      <c r="AO71" s="6"/>
+      <c r="AP71" s="6"/>
+      <c r="AQ71" s="6"/>
+      <c r="AR71" s="6"/>
       <c r="AS71" s="6"/>
       <c r="AT71" s="6"/>
       <c r="AU71" s="6"/>
@@ -4104,6 +4205,1254 @@
       <c r="AY72" s="4"/>
       <c r="AZ72" s="4"/>
     </row>
+    <row r="73">
+      <c r="A73" s="5"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
+      <c r="Q73" s="6"/>
+      <c r="R73" s="6"/>
+      <c r="S73" s="6"/>
+      <c r="T73" s="6"/>
+      <c r="U73" s="6"/>
+      <c r="V73" s="6"/>
+      <c r="W73" s="6"/>
+      <c r="X73" s="6"/>
+      <c r="Y73" s="6"/>
+      <c r="Z73" s="6"/>
+      <c r="AA73" s="6"/>
+      <c r="AB73" s="6"/>
+      <c r="AC73" s="6"/>
+      <c r="AD73" s="6"/>
+      <c r="AE73" s="6"/>
+      <c r="AF73" s="6"/>
+      <c r="AG73" s="6"/>
+      <c r="AH73" s="6"/>
+      <c r="AI73" s="6"/>
+      <c r="AJ73" s="6"/>
+      <c r="AK73" s="6"/>
+      <c r="AL73" s="6"/>
+      <c r="AM73" s="6"/>
+      <c r="AN73" s="6"/>
+      <c r="AO73" s="6"/>
+      <c r="AP73" s="6"/>
+      <c r="AQ73" s="6"/>
+      <c r="AR73" s="6"/>
+      <c r="AS73" s="6"/>
+      <c r="AT73" s="6"/>
+      <c r="AU73" s="6"/>
+      <c r="AV73" s="6"/>
+      <c r="AW73" s="6"/>
+      <c r="AX73" s="7"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="5"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="27"/>
+      <c r="J74" s="27"/>
+      <c r="K74" s="27"/>
+      <c r="L74" s="27"/>
+      <c r="M74" s="27"/>
+      <c r="N74" s="27"/>
+      <c r="O74" s="27"/>
+      <c r="P74" s="27"/>
+      <c r="Q74" s="27"/>
+      <c r="R74" s="27"/>
+      <c r="S74" s="27"/>
+      <c r="T74" s="27"/>
+      <c r="U74" s="27"/>
+      <c r="V74" s="27"/>
+      <c r="W74" s="27"/>
+      <c r="X74" s="27"/>
+      <c r="Y74" s="27"/>
+      <c r="Z74" s="6"/>
+      <c r="AA74" s="6"/>
+      <c r="AB74" s="6"/>
+      <c r="AC74" s="6"/>
+      <c r="AD74" s="6"/>
+      <c r="AE74" s="6"/>
+      <c r="AF74" s="6"/>
+      <c r="AG74" s="6"/>
+      <c r="AH74" s="6"/>
+      <c r="AI74" s="6"/>
+      <c r="AJ74" s="6"/>
+      <c r="AK74" s="6"/>
+      <c r="AL74" s="6"/>
+      <c r="AM74" s="6"/>
+      <c r="AN74" s="6"/>
+      <c r="AO74" s="6"/>
+      <c r="AP74" s="6"/>
+      <c r="AQ74" s="6"/>
+      <c r="AR74" s="6"/>
+      <c r="AS74" s="6"/>
+      <c r="AT74" s="6"/>
+      <c r="AU74" s="6"/>
+      <c r="AV74" s="15"/>
+      <c r="AW74" s="15"/>
+      <c r="AX74" s="21"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="5"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="27"/>
+      <c r="J75" s="27"/>
+      <c r="K75" s="27"/>
+      <c r="L75" s="27"/>
+      <c r="M75" s="27"/>
+      <c r="N75" s="27"/>
+      <c r="O75" s="27"/>
+      <c r="P75" s="27"/>
+      <c r="Q75" s="27"/>
+      <c r="R75" s="27"/>
+      <c r="S75" s="27"/>
+      <c r="T75" s="27"/>
+      <c r="U75" s="27"/>
+      <c r="V75" s="27"/>
+      <c r="W75" s="27"/>
+      <c r="X75" s="27"/>
+      <c r="Y75" s="27"/>
+      <c r="Z75" s="6"/>
+      <c r="AA75" s="6"/>
+      <c r="AB75" s="6"/>
+      <c r="AC75" s="6"/>
+      <c r="AD75" s="6"/>
+      <c r="AE75" s="6"/>
+      <c r="AF75" s="6"/>
+      <c r="AG75" s="6"/>
+      <c r="AH75" s="6"/>
+      <c r="AI75" s="6"/>
+      <c r="AJ75" s="6"/>
+      <c r="AK75" s="6"/>
+      <c r="AL75" s="6"/>
+      <c r="AM75" s="6"/>
+      <c r="AN75" s="6"/>
+      <c r="AO75" s="6"/>
+      <c r="AP75" s="6"/>
+      <c r="AQ75" s="6"/>
+      <c r="AR75" s="6"/>
+      <c r="AS75" s="6"/>
+      <c r="AT75" s="6"/>
+      <c r="AU75" s="6"/>
+      <c r="AV75" s="15"/>
+      <c r="AW75" s="15"/>
+      <c r="AX75" s="21"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="5"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="27"/>
+      <c r="J76" s="27"/>
+      <c r="K76" s="27"/>
+      <c r="L76" s="27"/>
+      <c r="M76" s="27"/>
+      <c r="N76" s="27"/>
+      <c r="O76" s="27"/>
+      <c r="P76" s="27"/>
+      <c r="Q76" s="27"/>
+      <c r="R76" s="27"/>
+      <c r="S76" s="27"/>
+      <c r="T76" s="27"/>
+      <c r="U76" s="27"/>
+      <c r="V76" s="27"/>
+      <c r="W76" s="27"/>
+      <c r="X76" s="27"/>
+      <c r="Y76" s="27"/>
+      <c r="Z76" s="6"/>
+      <c r="AA76" s="6"/>
+      <c r="AB76" s="6"/>
+      <c r="AC76" s="6"/>
+      <c r="AD76" s="6"/>
+      <c r="AE76" s="6"/>
+      <c r="AF76" s="6"/>
+      <c r="AG76" s="6"/>
+      <c r="AH76" s="6"/>
+      <c r="AI76" s="6"/>
+      <c r="AJ76" s="6"/>
+      <c r="AK76" s="6"/>
+      <c r="AL76" s="6"/>
+      <c r="AM76" s="6"/>
+      <c r="AN76" s="6"/>
+      <c r="AO76" s="6"/>
+      <c r="AP76" s="6"/>
+      <c r="AQ76" s="6"/>
+      <c r="AR76" s="6"/>
+      <c r="AS76" s="6"/>
+      <c r="AT76" s="6"/>
+      <c r="AU76" s="6"/>
+      <c r="AV76" s="15"/>
+      <c r="AW76" s="15"/>
+      <c r="AX76" s="21"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="5"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
+      <c r="Q77" s="6"/>
+      <c r="R77" s="6"/>
+      <c r="S77" s="6"/>
+      <c r="T77" s="6"/>
+      <c r="U77" s="6"/>
+      <c r="V77" s="6"/>
+      <c r="W77" s="6"/>
+      <c r="X77" s="6"/>
+      <c r="Y77" s="6"/>
+      <c r="Z77" s="6"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
+      <c r="AC77" s="6"/>
+      <c r="AD77" s="6"/>
+      <c r="AE77" s="6"/>
+      <c r="AF77" s="6"/>
+      <c r="AG77" s="6"/>
+      <c r="AH77" s="6"/>
+      <c r="AI77" s="6"/>
+      <c r="AJ77" s="6"/>
+      <c r="AK77" s="6"/>
+      <c r="AL77" s="6"/>
+      <c r="AM77" s="6"/>
+      <c r="AN77" s="6"/>
+      <c r="AO77" s="6"/>
+      <c r="AP77" s="6"/>
+      <c r="AQ77" s="6"/>
+      <c r="AR77" s="6"/>
+      <c r="AS77" s="6"/>
+      <c r="AT77" s="6"/>
+      <c r="AU77" s="6"/>
+      <c r="AV77" s="6"/>
+      <c r="AW77" s="6"/>
+      <c r="AX77" s="7"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="8"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="9"/>
+      <c r="R78" s="9"/>
+      <c r="S78" s="9"/>
+      <c r="T78" s="9"/>
+      <c r="U78" s="9"/>
+      <c r="V78" s="9"/>
+      <c r="W78" s="9"/>
+      <c r="X78" s="9"/>
+      <c r="Y78" s="9"/>
+      <c r="Z78" s="9"/>
+      <c r="AA78" s="9"/>
+      <c r="AB78" s="9"/>
+      <c r="AC78" s="9"/>
+      <c r="AD78" s="9"/>
+      <c r="AE78" s="9"/>
+      <c r="AF78" s="9"/>
+      <c r="AG78" s="9"/>
+      <c r="AH78" s="9"/>
+      <c r="AI78" s="9"/>
+      <c r="AJ78" s="9"/>
+      <c r="AK78" s="9"/>
+      <c r="AL78" s="9"/>
+      <c r="AM78" s="9"/>
+      <c r="AN78" s="9"/>
+      <c r="AO78" s="9"/>
+      <c r="AP78" s="9"/>
+      <c r="AQ78" s="9"/>
+      <c r="AR78" s="9"/>
+      <c r="AS78" s="9"/>
+      <c r="AT78" s="9"/>
+      <c r="AU78" s="9"/>
+      <c r="AV78" s="9"/>
+      <c r="AW78" s="9"/>
+      <c r="AX78" s="10"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="5"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
+      <c r="Q79" s="6"/>
+      <c r="R79" s="6"/>
+      <c r="S79" s="6"/>
+      <c r="T79" s="6"/>
+      <c r="U79" s="6"/>
+      <c r="V79" s="6"/>
+      <c r="W79" s="6"/>
+      <c r="X79" s="6"/>
+      <c r="Y79" s="6"/>
+      <c r="Z79" s="6"/>
+      <c r="AA79" s="6"/>
+      <c r="AB79" s="6"/>
+      <c r="AC79" s="6"/>
+      <c r="AD79" s="6"/>
+      <c r="AE79" s="6"/>
+      <c r="AF79" s="6"/>
+      <c r="AG79" s="6"/>
+      <c r="AH79" s="6"/>
+      <c r="AI79" s="6"/>
+      <c r="AJ79" s="6"/>
+      <c r="AK79" s="6"/>
+      <c r="AL79" s="6"/>
+      <c r="AM79" s="6"/>
+      <c r="AN79" s="6"/>
+      <c r="AO79" s="6"/>
+      <c r="AP79" s="6"/>
+      <c r="AQ79" s="6"/>
+      <c r="AR79" s="6"/>
+      <c r="AS79" s="6"/>
+      <c r="AT79" s="6"/>
+      <c r="AU79" s="6"/>
+      <c r="AV79" s="6"/>
+      <c r="AW79" s="6"/>
+      <c r="AX79" s="7"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="5"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+      <c r="P80" s="6"/>
+      <c r="Q80" s="6"/>
+      <c r="R80" s="6"/>
+      <c r="S80" s="6"/>
+      <c r="T80" s="6"/>
+      <c r="U80" s="22"/>
+      <c r="V80" s="22"/>
+      <c r="W80" s="22"/>
+      <c r="X80" s="22"/>
+      <c r="Y80" s="22"/>
+      <c r="Z80" s="22"/>
+      <c r="AA80" s="22"/>
+      <c r="AB80" s="22"/>
+      <c r="AC80" s="22"/>
+      <c r="AD80" s="6"/>
+      <c r="AE80" s="6"/>
+      <c r="AF80" s="6"/>
+      <c r="AG80" s="6"/>
+      <c r="AH80" s="6"/>
+      <c r="AI80" s="6"/>
+      <c r="AJ80" s="6"/>
+      <c r="AK80" s="6"/>
+      <c r="AL80" s="6"/>
+      <c r="AM80" s="6"/>
+      <c r="AN80" s="6"/>
+      <c r="AO80" s="6"/>
+      <c r="AP80" s="6"/>
+      <c r="AQ80" s="6"/>
+      <c r="AR80" s="6"/>
+      <c r="AS80" s="6"/>
+      <c r="AT80" s="6"/>
+      <c r="AU80" s="6"/>
+      <c r="AV80" s="15"/>
+      <c r="AW80" s="15"/>
+      <c r="AX80" s="21"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="5"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
+      <c r="Q81" s="6"/>
+      <c r="R81" s="6"/>
+      <c r="S81" s="6"/>
+      <c r="T81" s="6"/>
+      <c r="U81" s="22"/>
+      <c r="V81" s="22"/>
+      <c r="W81" s="22"/>
+      <c r="X81" s="22"/>
+      <c r="Y81" s="22"/>
+      <c r="Z81" s="22"/>
+      <c r="AA81" s="22"/>
+      <c r="AB81" s="22"/>
+      <c r="AC81" s="22"/>
+      <c r="AD81" s="6"/>
+      <c r="AE81" s="6"/>
+      <c r="AF81" s="6"/>
+      <c r="AG81" s="6"/>
+      <c r="AH81" s="6"/>
+      <c r="AI81" s="6"/>
+      <c r="AJ81" s="6"/>
+      <c r="AK81" s="6"/>
+      <c r="AL81" s="6"/>
+      <c r="AM81" s="6"/>
+      <c r="AN81" s="6"/>
+      <c r="AO81" s="6"/>
+      <c r="AP81" s="6"/>
+      <c r="AQ81" s="6"/>
+      <c r="AR81" s="6"/>
+      <c r="AS81" s="6"/>
+      <c r="AT81" s="6"/>
+      <c r="AU81" s="6"/>
+      <c r="AV81" s="15"/>
+      <c r="AW81" s="15"/>
+      <c r="AX81" s="21"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="5"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="6"/>
+      <c r="T82" s="6"/>
+      <c r="U82" s="22"/>
+      <c r="V82" s="22"/>
+      <c r="W82" s="22"/>
+      <c r="X82" s="22"/>
+      <c r="Y82" s="22"/>
+      <c r="Z82" s="22"/>
+      <c r="AA82" s="22"/>
+      <c r="AB82" s="22"/>
+      <c r="AC82" s="22"/>
+      <c r="AD82" s="6"/>
+      <c r="AE82" s="6"/>
+      <c r="AF82" s="6"/>
+      <c r="AG82" s="6"/>
+      <c r="AH82" s="6"/>
+      <c r="AI82" s="6"/>
+      <c r="AJ82" s="6"/>
+      <c r="AK82" s="6"/>
+      <c r="AL82" s="6"/>
+      <c r="AM82" s="6"/>
+      <c r="AN82" s="6"/>
+      <c r="AO82" s="6"/>
+      <c r="AP82" s="6"/>
+      <c r="AQ82" s="6"/>
+      <c r="AR82" s="6"/>
+      <c r="AS82" s="6"/>
+      <c r="AT82" s="6"/>
+      <c r="AU82" s="6"/>
+      <c r="AV82" s="15"/>
+      <c r="AW82" s="15"/>
+      <c r="AX82" s="21"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="5"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="6"/>
+      <c r="T83" s="6"/>
+      <c r="U83" s="6"/>
+      <c r="V83" s="6"/>
+      <c r="W83" s="6"/>
+      <c r="X83" s="6"/>
+      <c r="Y83" s="6"/>
+      <c r="Z83" s="6"/>
+      <c r="AA83" s="6"/>
+      <c r="AB83" s="6"/>
+      <c r="AC83" s="6"/>
+      <c r="AD83" s="6"/>
+      <c r="AE83" s="6"/>
+      <c r="AF83" s="6"/>
+      <c r="AG83" s="6"/>
+      <c r="AH83" s="6"/>
+      <c r="AI83" s="6"/>
+      <c r="AJ83" s="6"/>
+      <c r="AK83" s="6"/>
+      <c r="AL83" s="6"/>
+      <c r="AM83" s="6"/>
+      <c r="AN83" s="6"/>
+      <c r="AO83" s="6"/>
+      <c r="AP83" s="6"/>
+      <c r="AQ83" s="6"/>
+      <c r="AR83" s="6"/>
+      <c r="AS83" s="6"/>
+      <c r="AT83" s="6"/>
+      <c r="AU83" s="6"/>
+      <c r="AV83" s="6"/>
+      <c r="AW83" s="6"/>
+      <c r="AX83" s="7"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="8"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
+      <c r="O84" s="9"/>
+      <c r="P84" s="9"/>
+      <c r="Q84" s="9"/>
+      <c r="R84" s="9"/>
+      <c r="S84" s="9"/>
+      <c r="T84" s="9"/>
+      <c r="U84" s="9"/>
+      <c r="V84" s="9"/>
+      <c r="W84" s="9"/>
+      <c r="X84" s="9"/>
+      <c r="Y84" s="9"/>
+      <c r="Z84" s="9"/>
+      <c r="AA84" s="9"/>
+      <c r="AB84" s="9"/>
+      <c r="AC84" s="9"/>
+      <c r="AD84" s="9"/>
+      <c r="AE84" s="9"/>
+      <c r="AF84" s="9"/>
+      <c r="AG84" s="9"/>
+      <c r="AH84" s="9"/>
+      <c r="AI84" s="9"/>
+      <c r="AJ84" s="9"/>
+      <c r="AK84" s="9"/>
+      <c r="AL84" s="9"/>
+      <c r="AM84" s="9"/>
+      <c r="AN84" s="9"/>
+      <c r="AO84" s="9"/>
+      <c r="AP84" s="9"/>
+      <c r="AQ84" s="9"/>
+      <c r="AR84" s="9"/>
+      <c r="AS84" s="9"/>
+      <c r="AT84" s="9"/>
+      <c r="AU84" s="9"/>
+      <c r="AV84" s="9"/>
+      <c r="AW84" s="9"/>
+      <c r="AX84" s="10"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="5"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+      <c r="P85" s="6"/>
+      <c r="Q85" s="6"/>
+      <c r="R85" s="6"/>
+      <c r="S85" s="6"/>
+      <c r="T85" s="6"/>
+      <c r="U85" s="6"/>
+      <c r="V85" s="6"/>
+      <c r="W85" s="6"/>
+      <c r="X85" s="6"/>
+      <c r="Y85" s="6"/>
+      <c r="Z85" s="6"/>
+      <c r="AA85" s="6"/>
+      <c r="AB85" s="6"/>
+      <c r="AC85" s="6"/>
+      <c r="AD85" s="6"/>
+      <c r="AE85" s="6"/>
+      <c r="AF85" s="6"/>
+      <c r="AG85" s="6"/>
+      <c r="AH85" s="6"/>
+      <c r="AI85" s="6"/>
+      <c r="AJ85" s="6"/>
+      <c r="AK85" s="6"/>
+      <c r="AL85" s="6"/>
+      <c r="AM85" s="6"/>
+      <c r="AN85" s="6"/>
+      <c r="AO85" s="6"/>
+      <c r="AP85" s="6"/>
+      <c r="AQ85" s="6"/>
+      <c r="AR85" s="6"/>
+      <c r="AS85" s="6"/>
+      <c r="AT85" s="6"/>
+      <c r="AU85" s="6"/>
+      <c r="AV85" s="6"/>
+      <c r="AW85" s="6"/>
+      <c r="AX85" s="7"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="5"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+      <c r="O86" s="6"/>
+      <c r="P86" s="6"/>
+      <c r="Q86" s="6"/>
+      <c r="R86" s="6"/>
+      <c r="S86" s="6"/>
+      <c r="T86" s="6"/>
+      <c r="U86" s="6"/>
+      <c r="V86" s="6"/>
+      <c r="W86" s="6"/>
+      <c r="X86" s="6"/>
+      <c r="Y86" s="6"/>
+      <c r="Z86" s="6"/>
+      <c r="AA86" s="6"/>
+      <c r="AB86" s="6"/>
+      <c r="AC86" s="6"/>
+      <c r="AD86" s="6"/>
+      <c r="AE86" s="6"/>
+      <c r="AF86" s="6"/>
+      <c r="AG86" s="6"/>
+      <c r="AH86" s="6"/>
+      <c r="AI86" s="6"/>
+      <c r="AJ86" s="6"/>
+      <c r="AK86" s="6"/>
+      <c r="AL86" s="6"/>
+      <c r="AM86" s="6"/>
+      <c r="AN86" s="6"/>
+      <c r="AO86" s="6"/>
+      <c r="AP86" s="6"/>
+      <c r="AQ86" s="6"/>
+      <c r="AR86" s="6"/>
+      <c r="AS86" s="6"/>
+      <c r="AT86" s="6"/>
+      <c r="AU86" s="6"/>
+      <c r="AV86" s="15"/>
+      <c r="AW86" s="15"/>
+      <c r="AX86" s="21"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="5"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+      <c r="O87" s="6"/>
+      <c r="P87" s="6"/>
+      <c r="Q87" s="6"/>
+      <c r="R87" s="6"/>
+      <c r="S87" s="6"/>
+      <c r="T87" s="6"/>
+      <c r="U87" s="6"/>
+      <c r="V87" s="6"/>
+      <c r="W87" s="6"/>
+      <c r="X87" s="6"/>
+      <c r="Y87" s="6"/>
+      <c r="Z87" s="6"/>
+      <c r="AA87" s="6"/>
+      <c r="AB87" s="6"/>
+      <c r="AC87" s="6"/>
+      <c r="AD87" s="6"/>
+      <c r="AE87" s="6"/>
+      <c r="AF87" s="6"/>
+      <c r="AG87" s="6"/>
+      <c r="AH87" s="6"/>
+      <c r="AI87" s="6"/>
+      <c r="AJ87" s="6"/>
+      <c r="AK87" s="6"/>
+      <c r="AL87" s="6"/>
+      <c r="AM87" s="6"/>
+      <c r="AN87" s="6"/>
+      <c r="AO87" s="6"/>
+      <c r="AP87" s="6"/>
+      <c r="AQ87" s="6"/>
+      <c r="AR87" s="6"/>
+      <c r="AS87" s="6"/>
+      <c r="AT87" s="6"/>
+      <c r="AU87" s="6"/>
+      <c r="AV87" s="15"/>
+      <c r="AW87" s="15"/>
+      <c r="AX87" s="21"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="5"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
+      <c r="O88" s="6"/>
+      <c r="P88" s="6"/>
+      <c r="Q88" s="6"/>
+      <c r="R88" s="6"/>
+      <c r="S88" s="6"/>
+      <c r="T88" s="6"/>
+      <c r="U88" s="6"/>
+      <c r="V88" s="6"/>
+      <c r="W88" s="6"/>
+      <c r="X88" s="6"/>
+      <c r="Y88" s="6"/>
+      <c r="Z88" s="6"/>
+      <c r="AA88" s="6"/>
+      <c r="AB88" s="6"/>
+      <c r="AC88" s="6"/>
+      <c r="AD88" s="6"/>
+      <c r="AE88" s="6"/>
+      <c r="AF88" s="6"/>
+      <c r="AG88" s="6"/>
+      <c r="AH88" s="6"/>
+      <c r="AI88" s="6"/>
+      <c r="AJ88" s="6"/>
+      <c r="AK88" s="6"/>
+      <c r="AL88" s="6"/>
+      <c r="AM88" s="6"/>
+      <c r="AN88" s="6"/>
+      <c r="AO88" s="6"/>
+      <c r="AP88" s="6"/>
+      <c r="AQ88" s="6"/>
+      <c r="AR88" s="6"/>
+      <c r="AS88" s="6"/>
+      <c r="AT88" s="6"/>
+      <c r="AU88" s="6"/>
+      <c r="AV88" s="15"/>
+      <c r="AW88" s="15"/>
+      <c r="AX88" s="21"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="5"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="6"/>
+      <c r="N89" s="6"/>
+      <c r="O89" s="6"/>
+      <c r="P89" s="6"/>
+      <c r="Q89" s="6"/>
+      <c r="R89" s="6"/>
+      <c r="S89" s="6"/>
+      <c r="T89" s="6"/>
+      <c r="U89" s="6"/>
+      <c r="V89" s="6"/>
+      <c r="W89" s="6"/>
+      <c r="X89" s="6"/>
+      <c r="Y89" s="6"/>
+      <c r="Z89" s="6"/>
+      <c r="AA89" s="6"/>
+      <c r="AB89" s="6"/>
+      <c r="AC89" s="6"/>
+      <c r="AD89" s="6"/>
+      <c r="AE89" s="6"/>
+      <c r="AF89" s="6"/>
+      <c r="AG89" s="6"/>
+      <c r="AH89" s="6"/>
+      <c r="AI89" s="6"/>
+      <c r="AJ89" s="6"/>
+      <c r="AK89" s="6"/>
+      <c r="AL89" s="6"/>
+      <c r="AM89" s="6"/>
+      <c r="AN89" s="6"/>
+      <c r="AO89" s="6"/>
+      <c r="AP89" s="6"/>
+      <c r="AQ89" s="6"/>
+      <c r="AR89" s="6"/>
+      <c r="AS89" s="6"/>
+      <c r="AT89" s="6"/>
+      <c r="AU89" s="6"/>
+      <c r="AV89" s="6"/>
+      <c r="AW89" s="6"/>
+      <c r="AX89" s="7"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="8"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="9"/>
+      <c r="P90" s="9"/>
+      <c r="Q90" s="9"/>
+      <c r="R90" s="9"/>
+      <c r="S90" s="9"/>
+      <c r="T90" s="9"/>
+      <c r="U90" s="9"/>
+      <c r="V90" s="9"/>
+      <c r="W90" s="9"/>
+      <c r="X90" s="9"/>
+      <c r="Y90" s="9"/>
+      <c r="Z90" s="9"/>
+      <c r="AA90" s="9"/>
+      <c r="AB90" s="9"/>
+      <c r="AC90" s="9"/>
+      <c r="AD90" s="9"/>
+      <c r="AE90" s="9"/>
+      <c r="AF90" s="9"/>
+      <c r="AG90" s="9"/>
+      <c r="AH90" s="9"/>
+      <c r="AI90" s="9"/>
+      <c r="AJ90" s="9"/>
+      <c r="AK90" s="9"/>
+      <c r="AL90" s="9"/>
+      <c r="AM90" s="9"/>
+      <c r="AN90" s="9"/>
+      <c r="AO90" s="9"/>
+      <c r="AP90" s="9"/>
+      <c r="AQ90" s="9"/>
+      <c r="AR90" s="9"/>
+      <c r="AS90" s="9"/>
+      <c r="AT90" s="9"/>
+      <c r="AU90" s="9"/>
+      <c r="AV90" s="9"/>
+      <c r="AW90" s="9"/>
+      <c r="AX90" s="10"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="5"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
+      <c r="O91" s="6"/>
+      <c r="P91" s="6"/>
+      <c r="Q91" s="6"/>
+      <c r="R91" s="6"/>
+      <c r="S91" s="6"/>
+      <c r="T91" s="6"/>
+      <c r="U91" s="6"/>
+      <c r="V91" s="6"/>
+      <c r="W91" s="6"/>
+      <c r="X91" s="6"/>
+      <c r="Y91" s="6"/>
+      <c r="Z91" s="6"/>
+      <c r="AA91" s="6"/>
+      <c r="AB91" s="6"/>
+      <c r="AC91" s="6"/>
+      <c r="AD91" s="6"/>
+      <c r="AE91" s="6"/>
+      <c r="AF91" s="6"/>
+      <c r="AG91" s="6"/>
+      <c r="AH91" s="6"/>
+      <c r="AI91" s="6"/>
+      <c r="AJ91" s="6"/>
+      <c r="AK91" s="6"/>
+      <c r="AL91" s="6"/>
+      <c r="AM91" s="6"/>
+      <c r="AN91" s="6"/>
+      <c r="AO91" s="6"/>
+      <c r="AP91" s="6"/>
+      <c r="AQ91" s="6"/>
+      <c r="AR91" s="6"/>
+      <c r="AS91" s="6"/>
+      <c r="AT91" s="6"/>
+      <c r="AU91" s="6"/>
+      <c r="AV91" s="6"/>
+      <c r="AW91" s="6"/>
+      <c r="AX91" s="7"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="5"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+      <c r="O92" s="6"/>
+      <c r="P92" s="6"/>
+      <c r="Q92" s="6"/>
+      <c r="R92" s="6"/>
+      <c r="S92" s="6"/>
+      <c r="T92" s="6"/>
+      <c r="U92" s="6"/>
+      <c r="V92" s="6"/>
+      <c r="W92" s="6"/>
+      <c r="X92" s="6"/>
+      <c r="Y92" s="6"/>
+      <c r="Z92" s="6"/>
+      <c r="AA92" s="6"/>
+      <c r="AB92" s="6"/>
+      <c r="AC92" s="6"/>
+      <c r="AD92" s="6"/>
+      <c r="AE92" s="6"/>
+      <c r="AF92" s="6"/>
+      <c r="AG92" s="6"/>
+      <c r="AH92" s="6"/>
+      <c r="AI92" s="6"/>
+      <c r="AJ92" s="6"/>
+      <c r="AK92" s="6"/>
+      <c r="AL92" s="6"/>
+      <c r="AM92" s="6"/>
+      <c r="AN92" s="6"/>
+      <c r="AO92" s="6"/>
+      <c r="AP92" s="6"/>
+      <c r="AQ92" s="6"/>
+      <c r="AR92" s="6"/>
+      <c r="AS92" s="6"/>
+      <c r="AT92" s="6"/>
+      <c r="AU92" s="6"/>
+      <c r="AV92" s="15"/>
+      <c r="AW92" s="15"/>
+      <c r="AX92" s="21"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="5"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="6"/>
+      <c r="Q93" s="6"/>
+      <c r="R93" s="6"/>
+      <c r="S93" s="6"/>
+      <c r="T93" s="6"/>
+      <c r="U93" s="6"/>
+      <c r="V93" s="6"/>
+      <c r="W93" s="6"/>
+      <c r="X93" s="6"/>
+      <c r="Y93" s="6"/>
+      <c r="Z93" s="6"/>
+      <c r="AA93" s="6"/>
+      <c r="AB93" s="6"/>
+      <c r="AC93" s="6"/>
+      <c r="AD93" s="6"/>
+      <c r="AE93" s="6"/>
+      <c r="AF93" s="6"/>
+      <c r="AG93" s="6"/>
+      <c r="AH93" s="6"/>
+      <c r="AI93" s="6"/>
+      <c r="AJ93" s="6"/>
+      <c r="AK93" s="6"/>
+      <c r="AL93" s="6"/>
+      <c r="AM93" s="6"/>
+      <c r="AN93" s="6"/>
+      <c r="AO93" s="6"/>
+      <c r="AP93" s="6"/>
+      <c r="AQ93" s="6"/>
+      <c r="AR93" s="6"/>
+      <c r="AS93" s="6"/>
+      <c r="AT93" s="6"/>
+      <c r="AU93" s="6"/>
+      <c r="AV93" s="15"/>
+      <c r="AW93" s="15"/>
+      <c r="AX93" s="21"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="5"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+      <c r="O94" s="6"/>
+      <c r="P94" s="6"/>
+      <c r="Q94" s="6"/>
+      <c r="R94" s="6"/>
+      <c r="S94" s="6"/>
+      <c r="T94" s="6"/>
+      <c r="U94" s="6"/>
+      <c r="V94" s="6"/>
+      <c r="W94" s="6"/>
+      <c r="X94" s="6"/>
+      <c r="Y94" s="6"/>
+      <c r="Z94" s="6"/>
+      <c r="AA94" s="6"/>
+      <c r="AB94" s="6"/>
+      <c r="AC94" s="6"/>
+      <c r="AD94" s="6"/>
+      <c r="AE94" s="6"/>
+      <c r="AF94" s="6"/>
+      <c r="AG94" s="6"/>
+      <c r="AH94" s="6"/>
+      <c r="AI94" s="6"/>
+      <c r="AJ94" s="6"/>
+      <c r="AK94" s="6"/>
+      <c r="AL94" s="6"/>
+      <c r="AM94" s="6"/>
+      <c r="AN94" s="6"/>
+      <c r="AO94" s="6"/>
+      <c r="AP94" s="6"/>
+      <c r="AQ94" s="6"/>
+      <c r="AR94" s="6"/>
+      <c r="AS94" s="6"/>
+      <c r="AT94" s="6"/>
+      <c r="AU94" s="6"/>
+      <c r="AV94" s="15"/>
+      <c r="AW94" s="15"/>
+      <c r="AX94" s="21"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="5"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+      <c r="O95" s="6"/>
+      <c r="P95" s="6"/>
+      <c r="Q95" s="6"/>
+      <c r="R95" s="6"/>
+      <c r="S95" s="6"/>
+      <c r="T95" s="6"/>
+      <c r="U95" s="6"/>
+      <c r="V95" s="6"/>
+      <c r="W95" s="6"/>
+      <c r="X95" s="6"/>
+      <c r="Y95" s="6"/>
+      <c r="Z95" s="6"/>
+      <c r="AA95" s="6"/>
+      <c r="AB95" s="6"/>
+      <c r="AC95" s="6"/>
+      <c r="AD95" s="6"/>
+      <c r="AE95" s="6"/>
+      <c r="AF95" s="6"/>
+      <c r="AG95" s="6"/>
+      <c r="AH95" s="6"/>
+      <c r="AI95" s="6"/>
+      <c r="AJ95" s="6"/>
+      <c r="AK95" s="6"/>
+      <c r="AL95" s="6"/>
+      <c r="AM95" s="6"/>
+      <c r="AN95" s="6"/>
+      <c r="AO95" s="6"/>
+      <c r="AP95" s="6"/>
+      <c r="AQ95" s="6"/>
+      <c r="AR95" s="6"/>
+      <c r="AS95" s="6"/>
+      <c r="AT95" s="6"/>
+      <c r="AU95" s="6"/>
+      <c r="AV95" s="6"/>
+      <c r="AW95" s="6"/>
+      <c r="AX95" s="7"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="9"/>
+      <c r="K96" s="9"/>
+      <c r="L96" s="9"/>
+      <c r="M96" s="9"/>
+      <c r="N96" s="9"/>
+      <c r="O96" s="9"/>
+      <c r="P96" s="9"/>
+      <c r="Q96" s="9"/>
+      <c r="R96" s="9"/>
+      <c r="S96" s="9"/>
+      <c r="T96" s="9"/>
+      <c r="U96" s="9"/>
+      <c r="V96" s="9"/>
+      <c r="W96" s="9"/>
+      <c r="X96" s="9"/>
+      <c r="Y96" s="9"/>
+      <c r="Z96" s="9"/>
+      <c r="AA96" s="9"/>
+      <c r="AB96" s="9"/>
+      <c r="AC96" s="9"/>
+      <c r="AD96" s="9"/>
+      <c r="AE96" s="9"/>
+      <c r="AF96" s="9"/>
+      <c r="AG96" s="9"/>
+      <c r="AH96" s="9"/>
+      <c r="AI96" s="9"/>
+      <c r="AJ96" s="9"/>
+      <c r="AK96" s="9"/>
+      <c r="AL96" s="9"/>
+      <c r="AM96" s="9"/>
+      <c r="AN96" s="9"/>
+      <c r="AO96" s="9"/>
+      <c r="AP96" s="9"/>
+      <c r="AQ96" s="9"/>
+      <c r="AR96" s="9"/>
+      <c r="AS96" s="9"/>
+      <c r="AT96" s="9"/>
+      <c r="AU96" s="9"/>
+      <c r="AV96" s="9"/>
+      <c r="AW96" s="9"/>
+      <c r="AX96" s="10"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>